<commit_message>
Add 1st May as holiday in example 09
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -3947,8 +3947,8 @@
   </sheetPr>
   <dimension ref="A1:A49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3988,7 +3988,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="n">
-        <v>45658</v>
+        <v>45778</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,7 +4135,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add PM.Angel configuration to example 09
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -301,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="156">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -843,7 +843,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -853,7 +853,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD8CE"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFD7"/>
       </patternFill>
     </fill>
     <fill>
@@ -866,6 +866,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -903,7 +909,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -952,7 +958,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -964,6 +970,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -972,12 +982,28 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1029,7 +1055,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -1478,9 +1504,9 @@
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="13.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="22" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="27" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,11 +1522,11 @@
       <c r="D1" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="23" t="b">
+      <c r="E1" s="28" t="b">
         <f aca="false">AND(E2:E832)</f>
         <v>1</v>
       </c>
-      <c r="F1" s="23" t="b">
+      <c r="F1" s="28" t="b">
         <f aca="false">AND(F2:F832)</f>
         <v>1</v>
       </c>
@@ -1509,7 +1535,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -1518,11 +1544,11 @@
       <c r="D2" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E2" s="22" t="b">
+      <c r="E2" s="27" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F2" s="22" t="b">
+      <c r="F2" s="27" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B2) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1532,7 +1558,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -1541,11 +1567,11 @@
       <c r="D3" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E3" s="22" t="n">
+      <c r="E3" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F3" s="22" t="n">
+      <c r="F3" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B3) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1564,11 +1590,11 @@
       <c r="D4" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="E4" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F4" s="22" t="n">
+      <c r="F4" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B4) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1587,11 +1613,11 @@
       <c r="D5" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E5" s="22" t="n">
+      <c r="E5" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F5" s="22" t="n">
+      <c r="F5" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B5) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1610,11 +1636,11 @@
       <c r="D6" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E6" s="22" t="n">
+      <c r="E6" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F6" s="22" t="n">
+      <c r="F6" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B6) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1633,11 +1659,11 @@
       <c r="D7" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E7" s="22" t="n">
+      <c r="E7" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F7" s="22" t="n">
+      <c r="F7" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B7) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1656,11 +1682,11 @@
       <c r="D8" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E8" s="22" t="n">
+      <c r="E8" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F8" s="22" t="n">
+      <c r="F8" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B8) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1679,11 +1705,11 @@
       <c r="D9" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E9" s="22" t="n">
+      <c r="E9" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F9" s="22" t="n">
+      <c r="F9" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B9) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1702,11 +1728,11 @@
       <c r="D10" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E10" s="22" t="n">
+      <c r="E10" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F10" s="22" t="n">
+      <c r="F10" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B10) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1725,11 +1751,11 @@
       <c r="D11" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E11" s="22" t="n">
+      <c r="E11" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F11" s="22" t="n">
+      <c r="F11" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B11) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1748,11 +1774,11 @@
       <c r="D12" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E12" s="22" t="n">
+      <c r="E12" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A12) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F12" s="22" t="n">
+      <c r="F12" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B12) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1771,11 +1797,11 @@
       <c r="D13" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E13" s="22" t="n">
+      <c r="E13" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A13) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F13" s="22" t="n">
+      <c r="F13" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B13) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1785,7 +1811,7 @@
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -1794,11 +1820,11 @@
       <c r="D14" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E14" s="22" t="n">
+      <c r="E14" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A14) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F14" s="22" t="n">
+      <c r="F14" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B14) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1808,7 +1834,7 @@
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -1817,11 +1843,11 @@
       <c r="D15" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E15" s="22" t="n">
+      <c r="E15" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A15) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F15" s="22" t="n">
+      <c r="F15" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B15) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1840,11 +1866,11 @@
       <c r="D16" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E16" s="22" t="n">
+      <c r="E16" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A16) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F16" s="22" t="n">
+      <c r="F16" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B16) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1863,11 +1889,11 @@
       <c r="D17" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E17" s="22" t="n">
+      <c r="E17" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A17) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F17" s="22" t="n">
+      <c r="F17" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B17) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1886,11 +1912,11 @@
       <c r="D18" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E18" s="22" t="n">
+      <c r="E18" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A18) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F18" s="22" t="n">
+      <c r="F18" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B18) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1909,11 +1935,11 @@
       <c r="D19" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E19" s="22" t="n">
+      <c r="E19" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A19) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F19" s="22" t="n">
+      <c r="F19" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B19) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1932,11 +1958,11 @@
       <c r="D20" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E20" s="22" t="n">
+      <c r="E20" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A20) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F20" s="22" t="n">
+      <c r="F20" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B20) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1955,11 +1981,11 @@
       <c r="D21" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E21" s="22" t="n">
+      <c r="E21" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A21) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F21" s="22" t="n">
+      <c r="F21" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B21) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1978,11 +2004,11 @@
       <c r="D22" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E22" s="22" t="n">
+      <c r="E22" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A22) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F22" s="22" t="n">
+      <c r="F22" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B22) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2001,11 +2027,11 @@
       <c r="D23" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E23" s="22" t="n">
+      <c r="E23" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A23) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F23" s="22" t="n">
+      <c r="F23" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B23) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2024,11 +2050,11 @@
       <c r="D24" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E24" s="22" t="n">
+      <c r="E24" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A24) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F24" s="22" t="n">
+      <c r="F24" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B24) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2047,11 +2073,11 @@
       <c r="D25" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E25" s="22" t="n">
+      <c r="E25" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A25) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F25" s="22" t="n">
+      <c r="F25" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B25) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2061,7 +2087,7 @@
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C26" s="1" t="n">
@@ -2070,11 +2096,11 @@
       <c r="D26" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E26" s="22" t="n">
+      <c r="E26" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A26) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F26" s="22" t="n">
+      <c r="F26" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B26) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2084,7 +2110,7 @@
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C27" s="1" t="n">
@@ -2093,11 +2119,11 @@
       <c r="D27" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E27" s="22" t="n">
+      <c r="E27" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A27) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F27" s="22" t="n">
+      <c r="F27" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B27) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2116,11 +2142,11 @@
       <c r="D28" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E28" s="22" t="n">
+      <c r="E28" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A28) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F28" s="22" t="n">
+      <c r="F28" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B28) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2139,11 +2165,11 @@
       <c r="D29" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E29" s="22" t="n">
+      <c r="E29" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A29) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F29" s="22" t="n">
+      <c r="F29" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B29) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2162,11 +2188,11 @@
       <c r="D30" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E30" s="22" t="n">
+      <c r="E30" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A30) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F30" s="22" t="n">
+      <c r="F30" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B30) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2185,11 +2211,11 @@
       <c r="D31" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E31" s="22" t="n">
+      <c r="E31" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A31) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F31" s="22" t="n">
+      <c r="F31" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B31) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2208,11 +2234,11 @@
       <c r="D32" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E32" s="22" t="n">
+      <c r="E32" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A32) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F32" s="22" t="n">
+      <c r="F32" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B32) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2231,11 +2257,11 @@
       <c r="D33" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E33" s="22" t="n">
+      <c r="E33" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A33) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F33" s="22" t="n">
+      <c r="F33" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B33) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2254,11 +2280,11 @@
       <c r="D34" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E34" s="22" t="n">
+      <c r="E34" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A34) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F34" s="22" t="n">
+      <c r="F34" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B34) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2277,11 +2303,11 @@
       <c r="D35" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E35" s="22" t="n">
+      <c r="E35" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A35) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F35" s="22" t="n">
+      <c r="F35" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B35) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2300,11 +2326,11 @@
       <c r="D36" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E36" s="22" t="n">
+      <c r="E36" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A36) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F36" s="22" t="n">
+      <c r="F36" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B36) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2322,11 +2348,11 @@
       <c r="D37" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E37" s="22" t="n">
+      <c r="E37" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A37) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F37" s="22" t="n">
+      <c r="F37" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B37) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2335,7 +2361,7 @@
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C38" s="1" t="n">
@@ -2344,11 +2370,11 @@
       <c r="D38" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E38" s="22" t="n">
+      <c r="E38" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A38) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F38" s="22" t="n">
+      <c r="F38" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B38) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2357,7 +2383,7 @@
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C39" s="1" t="n">
@@ -2366,11 +2392,11 @@
       <c r="D39" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E39" s="22" t="n">
+      <c r="E39" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A39) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F39" s="22" t="n">
+      <c r="F39" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B39) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2388,11 +2414,11 @@
       <c r="D40" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E40" s="22" t="n">
+      <c r="E40" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A40) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F40" s="22" t="n">
+      <c r="F40" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B40) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2410,11 +2436,11 @@
       <c r="D41" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E41" s="22" t="n">
+      <c r="E41" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A41) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F41" s="22" t="n">
+      <c r="F41" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B41) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2432,11 +2458,11 @@
       <c r="D42" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E42" s="22" t="n">
+      <c r="E42" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A42) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F42" s="22" t="n">
+      <c r="F42" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B42) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2454,11 +2480,11 @@
       <c r="D43" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E43" s="22" t="n">
+      <c r="E43" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A43) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F43" s="22" t="n">
+      <c r="F43" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B43) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2476,11 +2502,11 @@
       <c r="D44" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E44" s="22" t="n">
+      <c r="E44" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A44) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F44" s="22" t="n">
+      <c r="F44" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B44) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2498,11 +2524,11 @@
       <c r="D45" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E45" s="22" t="n">
+      <c r="E45" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A45) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F45" s="22" t="n">
+      <c r="F45" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B45) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2520,11 +2546,11 @@
       <c r="D46" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E46" s="22" t="n">
+      <c r="E46" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A46) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F46" s="22" t="n">
+      <c r="F46" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B46) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2542,11 +2568,11 @@
       <c r="D47" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E47" s="22" t="n">
+      <c r="E47" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A47) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F47" s="22" t="n">
+      <c r="F47" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B47) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2564,11 +2590,11 @@
       <c r="D48" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E48" s="22" t="n">
+      <c r="E48" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A48) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F48" s="22" t="n">
+      <c r="F48" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B48) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2586,11 +2612,11 @@
       <c r="D49" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E49" s="22" t="n">
+      <c r="E49" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A49) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F49" s="22" t="n">
+      <c r="F49" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B49) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2599,7 +2625,7 @@
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C50" s="1" t="n">
@@ -2608,11 +2634,11 @@
       <c r="D50" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E50" s="22" t="n">
+      <c r="E50" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A50) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F50" s="22" t="n">
+      <c r="F50" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B50) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2621,7 +2647,7 @@
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C51" s="1" t="n">
@@ -2630,11 +2656,11 @@
       <c r="D51" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E51" s="22" t="n">
+      <c r="E51" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A51) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F51" s="22" t="n">
+      <c r="F51" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B51) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2652,11 +2678,11 @@
       <c r="D52" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E52" s="22" t="n">
+      <c r="E52" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A52) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F52" s="22" t="n">
+      <c r="F52" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B52) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2674,11 +2700,11 @@
       <c r="D53" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E53" s="22" t="n">
+      <c r="E53" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A53) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F53" s="22" t="n">
+      <c r="F53" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B53) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2696,11 +2722,11 @@
       <c r="D54" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E54" s="22" t="n">
+      <c r="E54" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A54) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F54" s="22" t="n">
+      <c r="F54" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B54) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2718,11 +2744,11 @@
       <c r="D55" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E55" s="22" t="n">
+      <c r="E55" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A55) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F55" s="22" t="n">
+      <c r="F55" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B55) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2740,11 +2766,11 @@
       <c r="D56" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E56" s="22" t="n">
+      <c r="E56" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A56) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F56" s="22" t="n">
+      <c r="F56" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B56) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2762,11 +2788,11 @@
       <c r="D57" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E57" s="22" t="n">
+      <c r="E57" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A57) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F57" s="22" t="n">
+      <c r="F57" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B57) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2784,11 +2810,11 @@
       <c r="D58" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E58" s="22" t="n">
+      <c r="E58" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A58) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F58" s="22" t="n">
+      <c r="F58" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B58) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2806,11 +2832,11 @@
       <c r="D59" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E59" s="22" t="n">
+      <c r="E59" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A59) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F59" s="22" t="n">
+      <c r="F59" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B59) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2828,11 +2854,11 @@
       <c r="D60" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E60" s="22" t="n">
+      <c r="E60" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A60) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F60" s="22" t="n">
+      <c r="F60" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B60) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2850,11 +2876,11 @@
       <c r="D61" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E61" s="22" t="n">
+      <c r="E61" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A61) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F61" s="22" t="n">
+      <c r="F61" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B61) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2863,7 +2889,7 @@
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B62" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C62" s="1" t="n">
@@ -2872,11 +2898,11 @@
       <c r="D62" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E62" s="22" t="n">
+      <c r="E62" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A62) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F62" s="22" t="n">
+      <c r="F62" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B62) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2885,7 +2911,7 @@
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C63" s="1" t="n">
@@ -2894,11 +2920,11 @@
       <c r="D63" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E63" s="22" t="n">
+      <c r="E63" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A63) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F63" s="22" t="n">
+      <c r="F63" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B63) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2916,11 +2942,11 @@
       <c r="D64" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E64" s="22" t="n">
+      <c r="E64" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A64) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F64" s="22" t="n">
+      <c r="F64" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B64) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2938,11 +2964,11 @@
       <c r="D65" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E65" s="22" t="n">
+      <c r="E65" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A65) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F65" s="22" t="n">
+      <c r="F65" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B65) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2960,11 +2986,11 @@
       <c r="D66" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E66" s="22" t="n">
+      <c r="E66" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A66) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F66" s="22" t="n">
+      <c r="F66" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B66) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2982,11 +3008,11 @@
       <c r="D67" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E67" s="22" t="n">
+      <c r="E67" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A67) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F67" s="22" t="n">
+      <c r="F67" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B67) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3004,11 +3030,11 @@
       <c r="D68" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E68" s="22" t="n">
+      <c r="E68" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A68) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F68" s="22" t="n">
+      <c r="F68" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B68) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3026,11 +3052,11 @@
       <c r="D69" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E69" s="22" t="n">
+      <c r="E69" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A69) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F69" s="22" t="n">
+      <c r="F69" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B69) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3048,11 +3074,11 @@
       <c r="D70" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E70" s="22" t="n">
+      <c r="E70" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A70) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F70" s="22" t="n">
+      <c r="F70" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B70) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3070,11 +3096,11 @@
       <c r="D71" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E71" s="22" t="n">
+      <c r="E71" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A71) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F71" s="22" t="n">
+      <c r="F71" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B71) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3092,11 +3118,11 @@
       <c r="D72" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E72" s="22" t="n">
+      <c r="E72" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A72) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F72" s="22" t="n">
+      <c r="F72" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B72) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3114,11 +3140,11 @@
       <c r="D73" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E73" s="22" t="n">
+      <c r="E73" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A73) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F73" s="22" t="n">
+      <c r="F73" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B73) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3127,7 +3153,7 @@
       <c r="A74" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="19" t="s">
+      <c r="B74" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C74" s="1" t="n">
@@ -3136,11 +3162,11 @@
       <c r="D74" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E74" s="22" t="n">
+      <c r="E74" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A74) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F74" s="22" t="n">
+      <c r="F74" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B74) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3149,7 +3175,7 @@
       <c r="A75" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B75" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C75" s="1" t="n">
@@ -3158,11 +3184,11 @@
       <c r="D75" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E75" s="22" t="n">
+      <c r="E75" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A75) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F75" s="22" t="n">
+      <c r="F75" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B75) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3180,11 +3206,11 @@
       <c r="D76" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E76" s="22" t="n">
+      <c r="E76" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A76) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F76" s="22" t="n">
+      <c r="F76" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B76) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3202,11 +3228,11 @@
       <c r="D77" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E77" s="22" t="n">
+      <c r="E77" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A77) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F77" s="22" t="n">
+      <c r="F77" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B77) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3224,11 +3250,11 @@
       <c r="D78" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E78" s="22" t="n">
+      <c r="E78" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A78) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F78" s="22" t="n">
+      <c r="F78" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B78) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3246,11 +3272,11 @@
       <c r="D79" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E79" s="22" t="n">
+      <c r="E79" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A79) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F79" s="22" t="n">
+      <c r="F79" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B79) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3268,11 +3294,11 @@
       <c r="D80" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E80" s="22" t="n">
+      <c r="E80" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A80) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F80" s="22" t="n">
+      <c r="F80" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B80) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3290,11 +3316,11 @@
       <c r="D81" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E81" s="22" t="n">
+      <c r="E81" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A81) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F81" s="22" t="n">
+      <c r="F81" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B81) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3312,11 +3338,11 @@
       <c r="D82" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E82" s="22" t="n">
+      <c r="E82" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A82) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F82" s="22" t="n">
+      <c r="F82" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B82) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3334,11 +3360,11 @@
       <c r="D83" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E83" s="22" t="n">
+      <c r="E83" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A83) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F83" s="22" t="n">
+      <c r="F83" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B83) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3356,11 +3382,11 @@
       <c r="D84" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E84" s="22" t="n">
+      <c r="E84" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A84) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F84" s="22" t="n">
+      <c r="F84" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B84) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3378,11 +3404,11 @@
       <c r="D85" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E85" s="22" t="n">
+      <c r="E85" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A85) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F85" s="22" t="n">
+      <c r="F85" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B85) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3391,7 +3417,7 @@
       <c r="A86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B86" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C86" s="1" t="n">
@@ -3400,11 +3426,11 @@
       <c r="D86" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E86" s="22" t="n">
+      <c r="E86" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A86) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F86" s="22" t="n">
+      <c r="F86" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B86) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3413,7 +3439,7 @@
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="B87" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C87" s="1" t="n">
@@ -3422,11 +3448,11 @@
       <c r="D87" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E87" s="22" t="n">
+      <c r="E87" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A87) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F87" s="22" t="n">
+      <c r="F87" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B87) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3444,11 +3470,11 @@
       <c r="D88" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E88" s="22" t="n">
+      <c r="E88" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A88) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F88" s="22" t="n">
+      <c r="F88" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B88) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3466,11 +3492,11 @@
       <c r="D89" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E89" s="22" t="n">
+      <c r="E89" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A89) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F89" s="22" t="n">
+      <c r="F89" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B89) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3488,11 +3514,11 @@
       <c r="D90" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E90" s="22" t="n">
+      <c r="E90" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A90) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F90" s="22" t="n">
+      <c r="F90" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B90) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3510,11 +3536,11 @@
       <c r="D91" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E91" s="22" t="n">
+      <c r="E91" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A91) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F91" s="22" t="n">
+      <c r="F91" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B91) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3532,11 +3558,11 @@
       <c r="D92" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E92" s="22" t="n">
+      <c r="E92" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A92) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F92" s="22" t="n">
+      <c r="F92" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B92) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3554,11 +3580,11 @@
       <c r="D93" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E93" s="22" t="n">
+      <c r="E93" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A93) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F93" s="22" t="n">
+      <c r="F93" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B93) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3576,11 +3602,11 @@
       <c r="D94" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E94" s="22" t="n">
+      <c r="E94" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A94) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F94" s="22" t="n">
+      <c r="F94" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B94) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3598,11 +3624,11 @@
       <c r="D95" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E95" s="22" t="n">
+      <c r="E95" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A95) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F95" s="22" t="n">
+      <c r="F95" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B95) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3620,11 +3646,11 @@
       <c r="D96" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E96" s="22" t="n">
+      <c r="E96" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A96) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F96" s="22" t="n">
+      <c r="F96" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B96) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3642,11 +3668,11 @@
       <c r="D97" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E97" s="22" t="n">
+      <c r="E97" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A97) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F97" s="22" t="n">
+      <c r="F97" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B97) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3655,7 +3681,7 @@
       <c r="A98" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B98" s="19" t="s">
+      <c r="B98" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C98" s="1" t="n">
@@ -3664,11 +3690,11 @@
       <c r="D98" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E98" s="22" t="n">
+      <c r="E98" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A98) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F98" s="22" t="n">
+      <c r="F98" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B98) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3677,7 +3703,7 @@
       <c r="A99" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B99" s="19" t="s">
+      <c r="B99" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C99" s="1" t="n">
@@ -3686,11 +3712,11 @@
       <c r="D99" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E99" s="22" t="n">
+      <c r="E99" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A99) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F99" s="22" t="n">
+      <c r="F99" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B99) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3708,11 +3734,11 @@
       <c r="D100" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E100" s="22" t="n">
+      <c r="E100" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A100) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F100" s="22" t="n">
+      <c r="F100" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B100) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3730,11 +3756,11 @@
       <c r="D101" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E101" s="22" t="n">
+      <c r="E101" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A101) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F101" s="22" t="n">
+      <c r="F101" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B101) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3752,11 +3778,11 @@
       <c r="D102" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E102" s="22" t="n">
+      <c r="E102" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A102) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F102" s="22" t="n">
+      <c r="F102" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B102) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3774,11 +3800,11 @@
       <c r="D103" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E103" s="22" t="n">
+      <c r="E103" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A103) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F103" s="22" t="n">
+      <c r="F103" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B103) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3796,11 +3822,11 @@
       <c r="D104" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E104" s="22" t="n">
+      <c r="E104" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A104) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F104" s="22" t="n">
+      <c r="F104" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B104) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3818,11 +3844,11 @@
       <c r="D105" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E105" s="22" t="n">
+      <c r="E105" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A105) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F105" s="22" t="n">
+      <c r="F105" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B105) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3840,11 +3866,11 @@
       <c r="D106" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E106" s="22" t="n">
+      <c r="E106" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A106) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F106" s="22" t="n">
+      <c r="F106" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B106) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3862,11 +3888,11 @@
       <c r="D107" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E107" s="22" t="n">
+      <c r="E107" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A107) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F107" s="22" t="n">
+      <c r="F107" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B107) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3884,11 +3910,11 @@
       <c r="D108" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E108" s="22" t="n">
+      <c r="E108" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A108) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F108" s="22" t="n">
+      <c r="F108" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B108) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3906,11 +3932,11 @@
       <c r="D109" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E109" s="22" t="n">
+      <c r="E109" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A109) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F109" s="22" t="n">
+      <c r="F109" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B109) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3919,7 +3945,7 @@
       <c r="A110" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B110" s="19" t="s">
+      <c r="B110" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C110" s="1" t="n">
@@ -3928,11 +3954,11 @@
       <c r="D110" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E110" s="22" t="n">
+      <c r="E110" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A110) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F110" s="22" t="n">
+      <c r="F110" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B110) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3941,7 +3967,7 @@
       <c r="A111" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="19" t="s">
+      <c r="B111" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C111" s="1" t="n">
@@ -3950,11 +3976,11 @@
       <c r="D111" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E111" s="22" t="n">
+      <c r="E111" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A111) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F111" s="22" t="n">
+      <c r="F111" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B111) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3972,11 +3998,11 @@
       <c r="D112" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E112" s="22" t="n">
+      <c r="E112" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A112) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F112" s="22" t="n">
+      <c r="F112" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B112) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3994,11 +4020,11 @@
       <c r="D113" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E113" s="22" t="n">
+      <c r="E113" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A113) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F113" s="22" t="n">
+      <c r="F113" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B113) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4016,11 +4042,11 @@
       <c r="D114" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E114" s="22" t="n">
+      <c r="E114" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A114) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F114" s="22" t="n">
+      <c r="F114" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B114) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4038,11 +4064,11 @@
       <c r="D115" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E115" s="22" t="n">
+      <c r="E115" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A115) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F115" s="22" t="n">
+      <c r="F115" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B115) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4060,11 +4086,11 @@
       <c r="D116" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E116" s="22" t="n">
+      <c r="E116" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A116) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F116" s="22" t="n">
+      <c r="F116" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B116) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4082,11 +4108,11 @@
       <c r="D117" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E117" s="22" t="n">
+      <c r="E117" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A117) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F117" s="22" t="n">
+      <c r="F117" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B117) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4104,11 +4130,11 @@
       <c r="D118" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E118" s="22" t="n">
+      <c r="E118" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A118) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F118" s="22" t="n">
+      <c r="F118" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B118) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4126,11 +4152,11 @@
       <c r="D119" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E119" s="22" t="n">
+      <c r="E119" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A119) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F119" s="22" t="n">
+      <c r="F119" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B119) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4148,11 +4174,11 @@
       <c r="D120" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E120" s="22" t="n">
+      <c r="E120" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A120) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F120" s="22" t="n">
+      <c r="F120" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B120) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4170,11 +4196,11 @@
       <c r="D121" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E121" s="22" t="n">
+      <c r="E121" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A121) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F121" s="22" t="n">
+      <c r="F121" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B121) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4183,7 +4209,7 @@
       <c r="A122" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B122" s="19" t="s">
+      <c r="B122" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C122" s="1" t="n">
@@ -4192,11 +4218,11 @@
       <c r="D122" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E122" s="22" t="n">
+      <c r="E122" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A122) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F122" s="22" t="n">
+      <c r="F122" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B122) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4205,7 +4231,7 @@
       <c r="A123" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B123" s="19" t="s">
+      <c r="B123" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C123" s="1" t="n">
@@ -4214,11 +4240,11 @@
       <c r="D123" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E123" s="22" t="n">
+      <c r="E123" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A123) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F123" s="22" t="n">
+      <c r="F123" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B123) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4236,11 +4262,11 @@
       <c r="D124" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E124" s="22" t="n">
+      <c r="E124" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A124) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F124" s="22" t="n">
+      <c r="F124" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B124) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4258,11 +4284,11 @@
       <c r="D125" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E125" s="22" t="n">
+      <c r="E125" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A125) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F125" s="22" t="n">
+      <c r="F125" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B125) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4280,11 +4306,11 @@
       <c r="D126" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E126" s="22" t="n">
+      <c r="E126" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A126) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F126" s="22" t="n">
+      <c r="F126" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B126) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4302,11 +4328,11 @@
       <c r="D127" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E127" s="22" t="n">
+      <c r="E127" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A127) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F127" s="22" t="n">
+      <c r="F127" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B127) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4324,11 +4350,11 @@
       <c r="D128" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E128" s="22" t="n">
+      <c r="E128" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A128) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F128" s="22" t="n">
+      <c r="F128" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B128) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4346,11 +4372,11 @@
       <c r="D129" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E129" s="22" t="n">
+      <c r="E129" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A129) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F129" s="22" t="n">
+      <c r="F129" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B129) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4368,11 +4394,11 @@
       <c r="D130" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E130" s="22" t="n">
+      <c r="E130" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A130) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F130" s="22" t="n">
+      <c r="F130" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B130) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4390,11 +4416,11 @@
       <c r="D131" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E131" s="22" t="n">
+      <c r="E131" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A131) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F131" s="22" t="n">
+      <c r="F131" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B131) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4412,11 +4438,11 @@
       <c r="D132" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E132" s="22" t="n">
+      <c r="E132" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A132) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F132" s="22" t="n">
+      <c r="F132" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B132) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4434,11 +4460,11 @@
       <c r="D133" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E133" s="22" t="n">
+      <c r="E133" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A133) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F133" s="22" t="n">
+      <c r="F133" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B133) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4447,7 +4473,7 @@
       <c r="A134" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B134" s="19" t="s">
+      <c r="B134" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C134" s="1" t="n">
@@ -4456,11 +4482,11 @@
       <c r="D134" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E134" s="22" t="n">
+      <c r="E134" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A134) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F134" s="22" t="n">
+      <c r="F134" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B134) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4469,7 +4495,7 @@
       <c r="A135" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B135" s="19" t="s">
+      <c r="B135" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C135" s="1" t="n">
@@ -4478,11 +4504,11 @@
       <c r="D135" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E135" s="22" t="n">
+      <c r="E135" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A135) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F135" s="22" t="n">
+      <c r="F135" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B135) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4500,11 +4526,11 @@
       <c r="D136" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E136" s="22" t="n">
+      <c r="E136" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A136) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F136" s="22" t="n">
+      <c r="F136" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B136) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4523,11 +4549,11 @@
       <c r="D137" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E137" s="22" t="n">
+      <c r="E137" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A137) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F137" s="22" t="n">
+      <c r="F137" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B137) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4546,11 +4572,11 @@
       <c r="D138" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E138" s="22" t="n">
+      <c r="E138" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A138) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F138" s="22" t="n">
+      <c r="F138" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B138) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4569,11 +4595,11 @@
       <c r="D139" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E139" s="22" t="n">
+      <c r="E139" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A139) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F139" s="22" t="n">
+      <c r="F139" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B139) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4592,11 +4618,11 @@
       <c r="D140" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E140" s="22" t="n">
+      <c r="E140" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A140) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F140" s="22" t="n">
+      <c r="F140" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B140) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4615,11 +4641,11 @@
       <c r="D141" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E141" s="22" t="n">
+      <c r="E141" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A141) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F141" s="22" t="n">
+      <c r="F141" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B141) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4638,11 +4664,11 @@
       <c r="D142" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E142" s="22" t="n">
+      <c r="E142" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A142) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F142" s="22" t="n">
+      <c r="F142" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B142) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4661,11 +4687,11 @@
       <c r="D143" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E143" s="22" t="n">
+      <c r="E143" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A143) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F143" s="22" t="n">
+      <c r="F143" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B143) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4684,11 +4710,11 @@
       <c r="D144" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E144" s="22" t="n">
+      <c r="E144" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A144) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F144" s="22" t="n">
+      <c r="F144" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B144) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4706,11 +4732,11 @@
       <c r="D145" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E145" s="22" t="n">
+      <c r="E145" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A145) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F145" s="22" t="n">
+      <c r="F145" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B145) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4719,7 +4745,7 @@
       <c r="A146" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B146" s="19" t="s">
+      <c r="B146" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C146" s="1" t="n">
@@ -4728,11 +4754,11 @@
       <c r="D146" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E146" s="22" t="n">
+      <c r="E146" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A146) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F146" s="22" t="n">
+      <c r="F146" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B146) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4741,7 +4767,7 @@
       <c r="A147" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B147" s="19" t="s">
+      <c r="B147" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C147" s="1" t="n">
@@ -4750,11 +4776,11 @@
       <c r="D147" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E147" s="22" t="n">
+      <c r="E147" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A147) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F147" s="22" t="n">
+      <c r="F147" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B147) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4772,11 +4798,11 @@
       <c r="D148" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E148" s="22" t="n">
+      <c r="E148" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A148) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F148" s="22" t="n">
+      <c r="F148" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B148) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4794,11 +4820,11 @@
       <c r="D149" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E149" s="22" t="n">
+      <c r="E149" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A149) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F149" s="22" t="n">
+      <c r="F149" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B149) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4816,11 +4842,11 @@
       <c r="D150" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E150" s="22" t="n">
+      <c r="E150" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A150) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F150" s="22" t="n">
+      <c r="F150" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B150) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4838,11 +4864,11 @@
       <c r="D151" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E151" s="22" t="n">
+      <c r="E151" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A151) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F151" s="22" t="n">
+      <c r="F151" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B151) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4860,11 +4886,11 @@
       <c r="D152" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E152" s="22" t="n">
+      <c r="E152" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A152) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F152" s="22" t="n">
+      <c r="F152" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B152) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4882,11 +4908,11 @@
       <c r="D153" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E153" s="22" t="n">
+      <c r="E153" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A153) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F153" s="22" t="n">
+      <c r="F153" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B153) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4904,11 +4930,11 @@
       <c r="D154" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E154" s="22" t="n">
+      <c r="E154" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A154) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F154" s="22" t="n">
+      <c r="F154" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B154) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4926,11 +4952,11 @@
       <c r="D155" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E155" s="22" t="n">
+      <c r="E155" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A155) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F155" s="22" t="n">
+      <c r="F155" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B155) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4948,11 +4974,11 @@
       <c r="D156" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E156" s="22" t="n">
+      <c r="E156" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A156) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F156" s="22" t="n">
+      <c r="F156" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B156) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4970,11 +4996,11 @@
       <c r="D157" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E157" s="22" t="n">
+      <c r="E157" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A157) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F157" s="22" t="n">
+      <c r="F157" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B157) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4983,7 +5009,7 @@
       <c r="A158" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B158" s="19" t="s">
+      <c r="B158" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C158" s="1" t="n">
@@ -4992,11 +5018,11 @@
       <c r="D158" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E158" s="22" t="n">
+      <c r="E158" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A158) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F158" s="22" t="n">
+      <c r="F158" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B158) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5005,7 +5031,7 @@
       <c r="A159" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B159" s="19" t="s">
+      <c r="B159" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C159" s="1" t="n">
@@ -5014,11 +5040,11 @@
       <c r="D159" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E159" s="22" t="n">
+      <c r="E159" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A159) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F159" s="22" t="n">
+      <c r="F159" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B159) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5036,11 +5062,11 @@
       <c r="D160" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E160" s="22" t="n">
+      <c r="E160" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A160) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F160" s="22" t="n">
+      <c r="F160" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B160) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5058,11 +5084,11 @@
       <c r="D161" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E161" s="22" t="n">
+      <c r="E161" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A161) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F161" s="22" t="n">
+      <c r="F161" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B161) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5080,11 +5106,11 @@
       <c r="D162" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E162" s="22" t="n">
+      <c r="E162" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A162) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F162" s="22" t="n">
+      <c r="F162" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B162) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5102,11 +5128,11 @@
       <c r="D163" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E163" s="22" t="n">
+      <c r="E163" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A163) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F163" s="22" t="n">
+      <c r="F163" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B163) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5124,11 +5150,11 @@
       <c r="D164" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E164" s="22" t="n">
+      <c r="E164" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A164) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F164" s="22" t="n">
+      <c r="F164" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B164) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5146,11 +5172,11 @@
       <c r="D165" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E165" s="22" t="n">
+      <c r="E165" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A165) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F165" s="22" t="n">
+      <c r="F165" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B165) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5168,11 +5194,11 @@
       <c r="D166" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E166" s="22" t="n">
+      <c r="E166" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A166) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F166" s="22" t="n">
+      <c r="F166" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B166) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5190,11 +5216,11 @@
       <c r="D167" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E167" s="22" t="n">
+      <c r="E167" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A167) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F167" s="22" t="n">
+      <c r="F167" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B167) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5212,11 +5238,11 @@
       <c r="D168" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E168" s="22" t="n">
+      <c r="E168" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A168) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F168" s="22" t="n">
+      <c r="F168" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B168) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5234,11 +5260,11 @@
       <c r="D169" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E169" s="22" t="n">
+      <c r="E169" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A169) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F169" s="22" t="n">
+      <c r="F169" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B169) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5247,7 +5273,7 @@
       <c r="A170" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B170" s="19" t="s">
+      <c r="B170" s="24" t="s">
         <v>133</v>
       </c>
       <c r="C170" s="1" t="n">
@@ -5256,11 +5282,11 @@
       <c r="D170" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E170" s="22" t="n">
+      <c r="E170" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A170) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F170" s="22" t="n">
+      <c r="F170" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B170) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5269,7 +5295,7 @@
       <c r="A171" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B171" s="19" t="s">
+      <c r="B171" s="24" t="s">
         <v>134</v>
       </c>
       <c r="C171" s="1" t="n">
@@ -5278,11 +5304,11 @@
       <c r="D171" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E171" s="22" t="n">
+      <c r="E171" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A171) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F171" s="22" t="n">
+      <c r="F171" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B171) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5300,11 +5326,11 @@
       <c r="D172" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E172" s="22" t="n">
+      <c r="E172" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A172) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F172" s="22" t="n">
+      <c r="F172" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B172) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5322,11 +5348,11 @@
       <c r="D173" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E173" s="22" t="n">
+      <c r="E173" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A173) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F173" s="22" t="n">
+      <c r="F173" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B173) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5344,11 +5370,11 @@
       <c r="D174" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E174" s="22" t="n">
+      <c r="E174" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A174) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F174" s="22" t="n">
+      <c r="F174" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B174) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5366,11 +5392,11 @@
       <c r="D175" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E175" s="22" t="n">
+      <c r="E175" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A175) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F175" s="22" t="n">
+      <c r="F175" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B175) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5388,11 +5414,11 @@
       <c r="D176" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E176" s="22" t="n">
+      <c r="E176" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A176) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F176" s="22" t="n">
+      <c r="F176" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B176) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5410,11 +5436,11 @@
       <c r="D177" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E177" s="22" t="n">
+      <c r="E177" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A177) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F177" s="22" t="n">
+      <c r="F177" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B177) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5432,11 +5458,11 @@
       <c r="D178" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E178" s="22" t="n">
+      <c r="E178" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A178) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F178" s="22" t="n">
+      <c r="F178" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B178) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5454,11 +5480,11 @@
       <c r="D179" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E179" s="22" t="n">
+      <c r="E179" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A179) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F179" s="22" t="n">
+      <c r="F179" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B179) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5476,11 +5502,11 @@
       <c r="D180" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E180" s="22" t="n">
+      <c r="E180" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A180) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F180" s="22" t="n">
+      <c r="F180" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B180) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5498,11 +5524,11 @@
       <c r="D181" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E181" s="22" t="n">
+      <c r="E181" s="27" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A181) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F181" s="22" t="n">
+      <c r="F181" s="27" t="n">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B181) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5761,16 +5787,16 @@
       <c r="C2" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="D2" s="17" t="n">
+      <c r="D2" s="12" t="n">
         <v>45658</v>
       </c>
-      <c r="E2" s="17" t="n">
+      <c r="E2" s="12" t="n">
         <v>46053</v>
       </c>
-      <c r="F2" s="17" t="n">
+      <c r="F2" s="12" t="n">
         <v>45658</v>
       </c>
-      <c r="G2" s="17" t="n">
+      <c r="G2" s="12" t="n">
         <v>46053</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -5795,7 +5821,7 @@
   </sheetPr>
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -10905,7 +10931,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10945,604 +10971,890 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="16" t="n">
         <v>45658</v>
       </c>
-      <c r="D2" s="15" t="n">
+      <c r="D2" s="16" t="n">
         <v>45748</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="16" t="b">
+      <c r="E2" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="17" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H2" s="16" t="b">
+      <c r="H2" s="17" t="b">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B2)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="16" t="n">
         <v>45749</v>
       </c>
-      <c r="D3" s="15" t="n">
+      <c r="D3" s="16" t="n">
         <v>45779</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="16" t="n">
+      <c r="E3" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H3" s="16" t="n">
+      <c r="H3" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B3)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="16" t="n">
         <v>45658</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="16" t="n">
         <v>45828</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="16" t="n">
+      <c r="E4" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H4" s="16" t="n">
+      <c r="H4" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B4)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="15" t="n">
+      <c r="C5" s="16" t="n">
         <v>45829</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="16" t="n">
         <v>45874</v>
       </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="16" t="n">
+      <c r="E5" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H5" s="16" t="n">
+      <c r="H5" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B5)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="15" t="n">
+      <c r="C6" s="16" t="n">
         <v>45658</v>
       </c>
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="16" t="n">
         <v>45931</v>
       </c>
-      <c r="E6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="16" t="n">
+      <c r="E6" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H6" s="16" t="n">
+      <c r="H6" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B6)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="15" t="n">
+      <c r="C7" s="16" t="n">
         <v>45932</v>
       </c>
-      <c r="D7" s="15" t="n">
+      <c r="D7" s="16" t="n">
         <v>45962</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="n">
+      <c r="E7" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="16" t="n">
+      <c r="G7" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H7" s="16" t="n">
+      <c r="H7" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B7)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="15" t="n">
+      <c r="C8" s="16" t="n">
         <v>45698</v>
       </c>
-      <c r="D8" s="15" t="n">
+      <c r="D8" s="16" t="n">
         <v>45715</v>
       </c>
-      <c r="E8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="16" t="n">
+      <c r="E8" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H8" s="16" t="n">
+      <c r="H8" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B8)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="15" t="n">
+      <c r="C9" s="16" t="n">
         <v>45717</v>
       </c>
-      <c r="D9" s="15" t="n">
+      <c r="D9" s="16" t="n">
         <v>45740</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="n">
+      <c r="E9" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="16" t="n">
+      <c r="G9" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H9" s="16" t="n">
+      <c r="H9" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B9)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="15" t="n">
+      <c r="C10" s="16" t="n">
         <v>45757</v>
       </c>
-      <c r="D10" s="15" t="n">
+      <c r="D10" s="16" t="n">
         <v>45767</v>
       </c>
-      <c r="E10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="n">
+      <c r="E10" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="16" t="n">
+      <c r="G10" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H10" s="16" t="n">
+      <c r="H10" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B10)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="15" t="n">
+      <c r="C11" s="16" t="n">
         <v>45803</v>
       </c>
-      <c r="D11" s="15" t="n">
+      <c r="D11" s="16" t="n">
         <v>45822</v>
       </c>
-      <c r="E11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="16" t="n">
+      <c r="E11" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H11" s="16" t="n">
+      <c r="H11" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B11)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="15" t="n">
+      <c r="C12" s="16" t="n">
         <v>45833</v>
       </c>
-      <c r="D12" s="15" t="n">
+      <c r="D12" s="16" t="n">
         <v>45847</v>
       </c>
-      <c r="E12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="n">
+      <c r="E12" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="16" t="n">
+      <c r="G12" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A12) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H12" s="16" t="n">
+      <c r="H12" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B12)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="15" t="n">
+      <c r="C13" s="16" t="n">
         <v>45833</v>
       </c>
-      <c r="D13" s="15" t="n">
+      <c r="D13" s="16" t="n">
         <v>45847</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="n">
+      <c r="E13" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="16" t="n">
+      <c r="G13" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A13) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H13" s="16" t="n">
+      <c r="H13" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B13)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="15" t="n">
+      <c r="C14" s="16" t="n">
         <v>45848</v>
       </c>
-      <c r="D14" s="15" t="n">
+      <c r="D14" s="16" t="n">
         <v>46021</v>
       </c>
-      <c r="E14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="16" t="n">
+      <c r="E14" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A14) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H14" s="16" t="n">
+      <c r="H14" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B14)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="15" t="n">
+      <c r="C15" s="16" t="n">
         <v>46022</v>
       </c>
-      <c r="D15" s="15" t="n">
+      <c r="D15" s="16" t="n">
         <v>46053</v>
       </c>
-      <c r="E15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="16" t="n">
+      <c r="E15" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="17" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A15) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="H15" s="16" t="n">
+      <c r="H15" s="17" t="n">
         <f aca="false">COUNTIF(tasks!$A$2:$A$906,B15)&gt;0</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="A16" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="19" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D16" s="19" t="n">
+        <v>45813</v>
+      </c>
+      <c r="E16" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A16) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B16)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="A17" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="19" t="n">
+        <v>45814</v>
+      </c>
+      <c r="D17" s="19" t="n">
+        <v>45844</v>
+      </c>
+      <c r="E17" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A17) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B17)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="A18" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="19" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D18" s="19" t="n">
+        <v>45713</v>
+      </c>
+      <c r="E18" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A18) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B18)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="A19" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="19" t="n">
+        <v>45714</v>
+      </c>
+      <c r="D19" s="19" t="n">
+        <v>45759</v>
+      </c>
+      <c r="E19" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A19) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B19)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="A20" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="19" t="n">
+        <v>45698</v>
+      </c>
+      <c r="D20" s="19" t="n">
+        <v>45715</v>
+      </c>
+      <c r="E20" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A20) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B20)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="A21" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="19" t="n">
+        <v>45716</v>
+      </c>
+      <c r="D21" s="19" t="n">
+        <v>45838</v>
+      </c>
+      <c r="E21" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A21) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B21)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="A22" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="19" t="n">
+        <v>45839</v>
+      </c>
+      <c r="D22" s="19" t="n">
+        <v>45884</v>
+      </c>
+      <c r="E22" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A22) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B22)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="A23" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="19" t="n">
+        <v>45757</v>
+      </c>
+      <c r="D23" s="19" t="n">
+        <v>45767</v>
+      </c>
+      <c r="E23" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A23) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H23" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B23)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="19" t="n">
+        <v>45768</v>
+      </c>
+      <c r="D24" s="19" t="n">
+        <v>45925</v>
+      </c>
+      <c r="E24" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A24) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H24" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B24)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="A25" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="19" t="n">
+        <v>45926</v>
+      </c>
+      <c r="D25" s="19" t="n">
+        <v>45960</v>
+      </c>
+      <c r="E25" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A25) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H25" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B25)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="A26" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="19" t="n">
+        <v>45803</v>
+      </c>
+      <c r="D26" s="19" t="n">
+        <v>45822</v>
+      </c>
+      <c r="E26" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A26) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B26)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="A27" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="19" t="n">
+        <v>45823</v>
+      </c>
+      <c r="D27" s="19" t="n">
+        <v>46021</v>
+      </c>
+      <c r="E27" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A27) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B27)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="A28" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="19" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D28" s="19" t="n">
+        <v>46053</v>
+      </c>
+      <c r="E28" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="17" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A28) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="17" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$906,B28)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
@@ -11727,8 +12039,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12091,7 +12403,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="U71" activeCellId="0" sqref="U71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12129,7 +12441,7 @@
       <c r="B2" s="6" t="n">
         <v>45658</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="C2" s="20" t="n">
         <v>46023</v>
       </c>
       <c r="D2" s="7" t="n">
@@ -12144,20 +12456,35 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="21" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C3" s="22" t="n">
+        <v>46023</v>
+      </c>
+      <c r="D3" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A3)&gt;0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
@@ -12612,28 +12939,28 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12975,8 +13302,8 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13014,7 +13341,7 @@
       <c r="B2" s="6" t="n">
         <v>45658</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="C2" s="20" t="n">
         <v>46023</v>
       </c>
       <c r="D2" s="7" t="n">
@@ -13029,8 +13356,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="21" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C3" s="22" t="n">
+        <v>46023</v>
+      </c>
+      <c r="D3" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A3) &gt; 0</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6"/>
@@ -13217,24 +13561,24 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="20" t="n">
+      <c r="B2" s="25" t="n">
         <v>45637</v>
       </c>
-      <c r="C2" s="20" t="n">
+      <c r="C2" s="25" t="n">
         <v>45672</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="25" t="n">
         <v>45673</v>
       </c>
-      <c r="C3" s="20" t="n">
+      <c r="C3" s="25" t="n">
         <v>45701</v>
       </c>
     </row>
@@ -13242,10 +13586,10 @@
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="18" t="n">
+      <c r="B4" s="20" t="n">
         <v>45702</v>
       </c>
-      <c r="C4" s="18" t="n">
+      <c r="C4" s="20" t="n">
         <v>45732</v>
       </c>
     </row>
@@ -13253,10 +13597,10 @@
       <c r="A5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="18" t="n">
+      <c r="B5" s="20" t="n">
         <v>45733</v>
       </c>
-      <c r="C5" s="18" t="n">
+      <c r="C5" s="20" t="n">
         <v>45761</v>
       </c>
     </row>
@@ -13264,10 +13608,10 @@
       <c r="A6" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="18" t="n">
+      <c r="B6" s="20" t="n">
         <v>45762</v>
       </c>
-      <c r="C6" s="18" t="n">
+      <c r="C6" s="20" t="n">
         <v>45795</v>
       </c>
     </row>
@@ -13275,10 +13619,10 @@
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="18" t="n">
+      <c r="B7" s="20" t="n">
         <v>45796</v>
       </c>
-      <c r="C7" s="18" t="n">
+      <c r="C7" s="20" t="n">
         <v>45826</v>
       </c>
     </row>
@@ -13289,7 +13633,7 @@
       <c r="B8" s="6" t="n">
         <v>45827</v>
       </c>
-      <c r="C8" s="18" t="n">
+      <c r="C8" s="20" t="n">
         <v>45855</v>
       </c>
     </row>
@@ -13297,10 +13641,10 @@
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="18" t="n">
+      <c r="B9" s="20" t="n">
         <v>45856</v>
       </c>
-      <c r="C9" s="18" t="n">
+      <c r="C9" s="20" t="n">
         <v>45886</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add additional checks in example 09
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="158">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -851,6 +851,21 @@
   </si>
   <si>
     <t xml:space="preserve">Solver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is T:start OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is T:end OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is H:start OK?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is H:end OK?</t>
   </si>
   <si>
     <t xml:space="preserve">highs</t>
@@ -921,7 +936,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -931,7 +946,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD8CE"/>
-        <bgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFD7D7"/>
       </patternFill>
     </fill>
     <fill>
@@ -950,6 +965,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFD7"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFD8CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -987,7 +1008,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1092,6 +1113,22 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,7 +1163,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -5804,10 +5841,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G59" activeCellId="0" sqref="G59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5815,6 +5852,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="19.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5842,6 +5884,21 @@
       <c r="H1" s="10" t="s">
         <v>151</v>
       </c>
+      <c r="I1" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
@@ -5866,7 +5923,27 @@
         <v>46053</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>152</v>
+        <v>157</v>
+      </c>
+      <c r="I2" s="27" t="n">
+        <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C900))</f>
+        <v>46053</v>
+      </c>
+      <c r="J2" s="28" t="n">
+        <f aca="false">AND(ISNUMBER(D2), D2&gt;A2)</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="29" t="b">
+        <f aca="false">AND(ISNUMBER(E2), E2&lt;=I2)</f>
+        <v>1</v>
+      </c>
+      <c r="L2" s="29" t="b">
+        <f aca="false">AND(ISNUMBER(F2), F2&gt;A2)</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="29" t="b">
+        <f aca="false">AND(ISNUMBER(G2), G2&lt;=I2)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -12501,7 +12578,7 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
In example 09 adjust constrains for PM.Lisa
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="158">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -1113,19 +1113,19 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1314,8 +1314,8 @@
   </sheetPr>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F67" activeCellId="0" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5843,7 +5843,7 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -5852,11 +5852,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="19.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="13.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12307,83 +12307,420 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="15"/>
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="12" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D29" s="12" t="n">
+        <v>45731</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A29) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H29" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B29)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C29), ISNUMBER(D29), C29&lt;=D29)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="12" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D30" s="12" t="n">
+        <v>45794</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A30) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B30)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C30), ISNUMBER(D30), C30&lt;=D30)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="12" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D31" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A31) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B31)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C31), ISNUMBER(D31), C31&lt;=D31)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="12" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D32" s="12" t="n">
+        <v>45779</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A32) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H32" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B32)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I32" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C32), ISNUMBER(D32), C32&lt;=D32)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="12" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D33" s="12" t="n">
+        <v>45789</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A33) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H33" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B33)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C33), ISNUMBER(D33), C33&lt;=D33)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="12" t="n">
+        <v>45790</v>
+      </c>
+      <c r="D34" s="12" t="n">
+        <v>45835</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A34) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B34)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I34" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C34), ISNUMBER(D34), C34&lt;=D34)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="12" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D35" s="12" t="n">
+        <v>45901</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A35) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B35)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I35" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C35), ISNUMBER(D35), C35&lt;=D35)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="12" t="n">
+        <v>45902</v>
+      </c>
+      <c r="D36" s="12" t="n">
+        <v>45947</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A36) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H36" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B36)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I36" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C36), ISNUMBER(D36), C36&lt;=D36)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="12" t="n">
+        <v>45717</v>
+      </c>
+      <c r="D37" s="12" t="n">
+        <v>45740</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A37) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H37" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B37)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I37" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C37), ISNUMBER(D37), C37&lt;=D37)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="12" t="n">
+        <v>45741</v>
+      </c>
+      <c r="D38" s="12" t="n">
+        <v>45870</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A38) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H38" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B38)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I38" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C38), ISNUMBER(D38), C38&lt;=D38)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="12" t="n">
+        <v>45871</v>
+      </c>
+      <c r="D39" s="12" t="n">
+        <v>45916</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A39) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B39)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I39" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C39), ISNUMBER(D39), C39&lt;=D39)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="12" t="n">
+        <v>45402</v>
+      </c>
+      <c r="D40" s="12" t="n">
+        <v>45962</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A40) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H40" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B40)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I40" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C40), ISNUMBER(D40), C40&lt;=D40)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="12" t="n">
+        <v>45963</v>
+      </c>
+      <c r="D41" s="12" t="n">
+        <v>45991</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A41) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B41)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I41" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C41), ISNUMBER(D41), C41&lt;=D41)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="12"/>
@@ -13000,7 +13337,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13087,10 +13424,29 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C4" s="12" t="n">
+        <v>46002</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A4)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="12"/>

</xml_diff>

<commit_message>
In exaple 09 add constrains for DEVs
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="158">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -868,7 +868,7 @@
     <t xml:space="preserve">Is H:end OK?</t>
   </si>
   <si>
-    <t xml:space="preserve">highs</t>
+    <t xml:space="preserve">scip</t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1314,8 @@
   </sheetPr>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F67" activeCellId="0" sqref="F67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5843,8 +5843,8 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13334,10 +13334,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13397,6 +13397,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="19"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
@@ -13449,64 +13450,256 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="20" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C5" s="21" t="n">
+        <f aca="false">B5+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A5)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C6" s="12" t="n">
+        <f aca="false">B6+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A6)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="20" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C7" s="21" t="n">
+        <f aca="false">B7+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D7" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A7)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B7), ISNUMBER(C7), B7&lt;=C7)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C8" s="12" t="n">
+        <f aca="false">B8+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A8)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B8), ISNUMBER(C8), B8&lt;=C8)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="20" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C9" s="21" t="n">
+        <f aca="false">B9+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A9)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B9), ISNUMBER(C9), B9&lt;=C9)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C10" s="12" t="n">
+        <f aca="false">B10+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A10)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B10), ISNUMBER(C10), B10&lt;=C10)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="20" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C11" s="21" t="n">
+        <f aca="false">B11+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D11" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A11)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B11), ISNUMBER(C11), B11&lt;=C11)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C12" s="12" t="n">
+        <f aca="false">B12+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A12)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B12), ISNUMBER(C12), B12&lt;=C12)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="20" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C13" s="21" t="n">
+        <f aca="false">B13+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D13" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987,A13)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(B13), ISNUMBER(C13), B13&lt;=C13)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C14" s="12" t="n">
+        <f aca="false">B14+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>

</xml_diff>

<commit_message>
In example 09 add constrains for SA.Adrian and SA.Robert
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="158">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -868,7 +868,7 @@
     <t xml:space="preserve">Is H:end OK?</t>
   </si>
   <si>
-    <t xml:space="preserve">scip</t>
+    <t xml:space="preserve">highs</t>
   </si>
 </sst>
 </file>
@@ -881,7 +881,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -927,12 +927,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1008,7 +1002,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1081,14 +1075,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1099,6 +1085,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1315,7 +1305,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1607,7 +1597,7 @@
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="13.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="11.57"/>
   </cols>
@@ -1638,7 +1628,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -1661,7 +1651,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -1914,7 +1904,7 @@
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -1937,7 +1927,7 @@
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -2190,7 +2180,7 @@
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C26" s="1" t="n">
@@ -2213,7 +2203,7 @@
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C27" s="1" t="n">
@@ -2464,7 +2454,7 @@
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C38" s="1" t="n">
@@ -2486,7 +2476,7 @@
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C39" s="1" t="n">
@@ -2728,7 +2718,7 @@
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="23" t="s">
+      <c r="B50" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C50" s="1" t="n">
@@ -2750,7 +2740,7 @@
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C51" s="1" t="n">
@@ -2992,7 +2982,7 @@
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="23" t="s">
+      <c r="B62" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C62" s="1" t="n">
@@ -3014,7 +3004,7 @@
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="23" t="s">
+      <c r="B63" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C63" s="1" t="n">
@@ -3256,7 +3246,7 @@
       <c r="A74" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="23" t="s">
+      <c r="B74" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C74" s="1" t="n">
@@ -3278,7 +3268,7 @@
       <c r="A75" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="23" t="s">
+      <c r="B75" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C75" s="1" t="n">
@@ -3520,7 +3510,7 @@
       <c r="A86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C86" s="1" t="n">
@@ -3542,7 +3532,7 @@
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="23" t="s">
+      <c r="B87" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C87" s="1" t="n">
@@ -3784,7 +3774,7 @@
       <c r="A98" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B98" s="23" t="s">
+      <c r="B98" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C98" s="1" t="n">
@@ -3806,7 +3796,7 @@
       <c r="A99" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B99" s="23" t="s">
+      <c r="B99" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C99" s="1" t="n">
@@ -4048,7 +4038,7 @@
       <c r="A110" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B110" s="23" t="s">
+      <c r="B110" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C110" s="1" t="n">
@@ -4070,7 +4060,7 @@
       <c r="A111" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="23" t="s">
+      <c r="B111" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C111" s="1" t="n">
@@ -4312,7 +4302,7 @@
       <c r="A122" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B122" s="23" t="s">
+      <c r="B122" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C122" s="1" t="n">
@@ -4334,7 +4324,7 @@
       <c r="A123" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B123" s="23" t="s">
+      <c r="B123" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C123" s="1" t="n">
@@ -4576,7 +4566,7 @@
       <c r="A134" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B134" s="23" t="s">
+      <c r="B134" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C134" s="1" t="n">
@@ -4598,7 +4588,7 @@
       <c r="A135" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B135" s="23" t="s">
+      <c r="B135" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C135" s="1" t="n">
@@ -4848,7 +4838,7 @@
       <c r="A146" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B146" s="23" t="s">
+      <c r="B146" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C146" s="1" t="n">
@@ -4870,7 +4860,7 @@
       <c r="A147" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B147" s="23" t="s">
+      <c r="B147" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C147" s="1" t="n">
@@ -5112,7 +5102,7 @@
       <c r="A158" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B158" s="23" t="s">
+      <c r="B158" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C158" s="1" t="n">
@@ -5134,7 +5124,7 @@
       <c r="A159" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B159" s="23" t="s">
+      <c r="B159" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C159" s="1" t="n">
@@ -5376,7 +5366,7 @@
       <c r="A170" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B170" s="23" t="s">
+      <c r="B170" s="22" t="s">
         <v>130</v>
       </c>
       <c r="C170" s="1" t="n">
@@ -5398,7 +5388,7 @@
       <c r="A171" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B171" s="23" t="s">
+      <c r="B171" s="22" t="s">
         <v>131</v>
       </c>
       <c r="C171" s="1" t="n">
@@ -5843,7 +5833,7 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -5884,19 +5874,19 @@
       <c r="H1" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="25" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5925,23 +5915,23 @@
       <c r="H2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I2" s="27" t="n">
+      <c r="I2" s="26" t="n">
         <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C900))</f>
         <v>46053</v>
       </c>
-      <c r="J2" s="28" t="n">
+      <c r="J2" s="27" t="n">
         <f aca="false">AND(ISNUMBER(D2), D2&gt;A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="29" t="b">
+      <c r="K2" s="28" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&lt;=I2)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="29" t="b">
+      <c r="L2" s="28" t="b">
         <f aca="false">AND(ISNUMBER(F2), F2&gt;A2)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="29" t="b">
+      <c r="M2" s="28" t="b">
         <f aca="false">AND(ISNUMBER(G2), G2&lt;=I2)</f>
         <v>1</v>
       </c>
@@ -5964,8 +5954,8 @@
   </sheetPr>
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A100" activeCellId="0" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11396,10 +11386,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11430,15 +11420,15 @@
         <v>129</v>
       </c>
       <c r="G1" s="5" t="b">
-        <f aca="false">AND(G2:G938)</f>
+        <f aca="false">AND(G2:G937)</f>
         <v>1</v>
       </c>
       <c r="H1" s="5" t="b">
-        <f aca="false">AND(H2:H938)</f>
+        <f aca="false">AND(H2:H937)</f>
         <v>1</v>
       </c>
       <c r="I1" s="11" t="b">
-        <f aca="false">AND(I2:I908)</f>
+        <f aca="false">AND(I2:I907)</f>
         <v>1</v>
       </c>
     </row>
@@ -12723,94 +12713,484 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="A42" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="17" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D42" s="17" t="n">
+        <v>45779</v>
+      </c>
+      <c r="E42" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F42" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G42" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A42) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H42" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B42)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I42" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C42), ISNUMBER(D42), C42&lt;=D42)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="A43" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="17" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D43" s="17" t="n">
+        <v>45813</v>
+      </c>
+      <c r="E43" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A43) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H43" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B43)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I43" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C43), ISNUMBER(D43), C43&lt;=D43)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="A44" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="17" t="n">
+        <v>45814</v>
+      </c>
+      <c r="D44" s="17" t="n">
+        <v>45844</v>
+      </c>
+      <c r="E44" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A44) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H44" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B44)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I44" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C44), ISNUMBER(D44), C44&lt;=D44)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="A45" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="17" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D45" s="17" t="n">
+        <v>45731</v>
+      </c>
+      <c r="E45" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A45) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B45)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I45" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C45), ISNUMBER(D45), C45&lt;=D45)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="A46" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="17" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D46" s="17" t="n">
+        <v>45794</v>
+      </c>
+      <c r="E46" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A46) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H46" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B46)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I46" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C46), ISNUMBER(D46), C46&lt;=D46)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="A47" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="17" t="n">
+        <v>45790</v>
+      </c>
+      <c r="D47" s="17" t="n">
+        <v>45835</v>
+      </c>
+      <c r="E47" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A47) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H47" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B47)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I47" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C47), ISNUMBER(D47), C47&lt;=D47)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="12" t="n">
+        <v>45829</v>
+      </c>
+      <c r="D48" s="12" t="n">
+        <v>45874</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A48) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H48" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B48)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I48" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C48), ISNUMBER(D48), C48&lt;=D48)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="A49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="12" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D49" s="12" t="n">
+        <v>45748</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A49) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H49" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B49)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I49" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C49), ISNUMBER(D49), C49&lt;=D49)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="12" t="n">
+        <v>45749</v>
+      </c>
+      <c r="D50" s="12" t="n">
+        <v>45779</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A50) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H50" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B50)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I50" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C50), ISNUMBER(D50), C50&lt;=D50)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="12" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D51" s="12" t="n">
+        <v>45789</v>
+      </c>
+      <c r="E51" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A51) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H51" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B51)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I51" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C51), ISNUMBER(D51), C51&lt;=D51)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="12" t="n">
+        <v>45790</v>
+      </c>
+      <c r="D52" s="12" t="n">
+        <v>45835</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A52) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H52" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B52)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I52" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C52), ISNUMBER(D52), C52&lt;=D52)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="12" t="n">
+        <v>45658</v>
+      </c>
+      <c r="D53" s="12" t="n">
+        <v>45901</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A53) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H53" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B53)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I53" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C53), ISNUMBER(D53), C53&lt;=D53)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="12" t="n">
+        <v>45902</v>
+      </c>
+      <c r="D54" s="12" t="n">
+        <v>45947</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A54) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H54" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B54)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I54" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C54), ISNUMBER(D54), C54&lt;=D54)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="12" t="n">
+        <v>45932</v>
+      </c>
+      <c r="D55" s="12" t="n">
+        <v>45962</v>
+      </c>
+      <c r="E55" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A55) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H55" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B55)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I55" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C55), ISNUMBER(D55), C55&lt;=D55)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="12" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D56" s="12" t="n">
+        <v>46053</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" s="15" t="n">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A56) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="H56" s="15" t="n">
+        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B56)&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="I56" s="15" t="n">
+        <f aca="false">AND(ISNUMBER(C56), ISNUMBER(D56), C56&lt;=D56)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="1"/>
@@ -12890,12 +13270,7 @@
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -13334,10 +13709,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13364,29 +13739,30 @@
         <v>129</v>
       </c>
       <c r="F1" s="5" t="b">
-        <f aca="false">AND(F2:F938)</f>
+        <f aca="false">AND(F2:F935)</f>
         <v>1</v>
       </c>
       <c r="G1" s="11" t="b">
-        <f aca="false">AND(G2:G908)</f>
+        <f aca="false">AND(G2:G905)</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6" t="n">
+      <c r="A2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="18" t="n">
         <v>45658</v>
       </c>
-      <c r="C2" s="18" t="n">
-        <v>46023</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <v>2</v>
+      <c r="C2" s="19" t="n">
+        <f aca="false">B2+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D2" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="20" t="n">
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A2)&gt;0</f>
@@ -13396,24 +13772,23 @@
         <f aca="false">AND(ISNUMBER(B2), ISNUMBER(C2), B2&lt;=C2)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="K2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="20" t="n">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>45658</v>
       </c>
-      <c r="C3" s="21" t="n">
-        <v>46023</v>
-      </c>
-      <c r="D3" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="22" t="n">
-        <v>2</v>
+      <c r="C3" s="12" t="n">
+        <f aca="false">B3+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A3)&gt;0</f>
@@ -13425,97 +13800,98 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="12" t="n">
+      <c r="A4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="18" t="n">
         <v>45658</v>
       </c>
-      <c r="C4" s="12" t="n">
-        <v>46002</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2" t="b">
+      <c r="C4" s="19" t="n">
+        <f aca="false">B4+20</f>
+        <v>45678</v>
+      </c>
+      <c r="D4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A4)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="G4" s="2" t="b">
+      <c r="G4" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="20" t="n">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>45658</v>
       </c>
-      <c r="C5" s="21" t="n">
+      <c r="C5" s="12" t="n">
         <f aca="false">B5+20</f>
         <v>45678</v>
       </c>
-      <c r="D5" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="b">
+      <c r="D5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A5)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="b">
+      <c r="G5" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B5), ISNUMBER(C5), B5&lt;=C5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6" t="n">
+      <c r="A6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="18" t="n">
         <v>45658</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="19" t="n">
         <f aca="false">B6+20</f>
         <v>45678</v>
       </c>
-      <c r="D6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="b">
+      <c r="D6" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$987,A6)&gt;0</f>
         <v>1</v>
       </c>
-      <c r="G6" s="2" t="b">
+      <c r="G6" s="2" t="n">
         <f aca="false">AND(ISNUMBER(B6), ISNUMBER(C6), B6&lt;=C6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="20" t="n">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="n">
         <v>45658</v>
       </c>
-      <c r="C7" s="21" t="n">
+      <c r="C7" s="12" t="n">
         <f aca="false">B7+20</f>
         <v>45678</v>
       </c>
-      <c r="D7" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="22" t="n">
+      <c r="D7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="n">
@@ -13528,20 +13904,20 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="6" t="n">
+      <c r="A8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="18" t="n">
         <v>45658</v>
       </c>
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="19" t="n">
         <f aca="false">B8+20</f>
         <v>45678</v>
       </c>
-      <c r="D8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7" t="n">
+      <c r="D8" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="20" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="n">
@@ -13554,20 +13930,20 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="20" t="n">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="n">
         <v>45658</v>
       </c>
-      <c r="C9" s="21" t="n">
+      <c r="C9" s="12" t="n">
         <f aca="false">B9+20</f>
         <v>45678</v>
       </c>
-      <c r="D9" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="22" t="n">
+      <c r="D9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="n">
@@ -13580,20 +13956,20 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="6" t="n">
+      <c r="A10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="18" t="n">
         <v>45658</v>
       </c>
-      <c r="C10" s="12" t="n">
+      <c r="C10" s="19" t="n">
         <f aca="false">B10+20</f>
         <v>45678</v>
       </c>
-      <c r="D10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7" t="n">
+      <c r="D10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="20" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="n">
@@ -13606,100 +13982,40 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="20" t="n">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6" t="n">
         <v>45658</v>
       </c>
-      <c r="C11" s="21" t="n">
+      <c r="C11" s="12" t="n">
         <f aca="false">B11+20</f>
         <v>45678</v>
       </c>
-      <c r="D11" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <f aca="false">COUNTIF(experts!$A$2:$A$987,A11)&gt;0</f>
-        <v>1</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(B11), ISNUMBER(C11), B11&lt;=C11)</f>
+      <c r="D11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>45658</v>
-      </c>
-      <c r="C12" s="12" t="n">
-        <f aca="false">B12+20</f>
-        <v>45678</v>
-      </c>
-      <c r="D12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <f aca="false">COUNTIF(experts!$A$2:$A$987,A12)&gt;0</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(B12), ISNUMBER(C12), B12&lt;=C12)</f>
-        <v>1</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="20" t="n">
-        <v>45658</v>
-      </c>
-      <c r="C13" s="21" t="n">
-        <f aca="false">B13+20</f>
-        <v>45678</v>
-      </c>
-      <c r="D13" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <f aca="false">COUNTIF(experts!$A$2:$A$987,A13)&gt;0</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(B13), ISNUMBER(C13), B13&lt;=C13)</f>
-        <v>1</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6" t="n">
-        <v>45658</v>
-      </c>
-      <c r="C14" s="12" t="n">
-        <f aca="false">B14+20</f>
-        <v>45678</v>
-      </c>
-      <c r="D14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1"/>
@@ -14019,24 +14335,9 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -14478,7 +14779,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14520,7 +14821,7 @@
       <c r="B2" s="6" t="n">
         <v>45658</v>
       </c>
-      <c r="C2" s="18" t="n">
+      <c r="C2" s="21" t="n">
         <v>46023</v>
       </c>
       <c r="D2" s="7" t="n">
@@ -14542,16 +14843,16 @@
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20" t="n">
+      <c r="B3" s="18" t="n">
         <v>45658</v>
       </c>
-      <c r="C3" s="21" t="n">
+      <c r="C3" s="19" t="n">
         <v>46023</v>
       </c>
-      <c r="D3" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="22" t="n">
+      <c r="D3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="20" t="n">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="b">
@@ -14564,8 +14865,29 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>45658</v>
+      </c>
+      <c r="C4" s="21" t="n">
+        <v>46023</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="b">
+        <f aca="false">COUNTIF(experts!$A$2:$A$987, A4) &gt; 0</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <f aca="false">AND(ISNUMBER(B4), ISNUMBER(C4), B4&lt;=C4)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6"/>
@@ -14753,13 +15075,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="24" t="n">
+      <c r="B2" s="23" t="n">
         <v>45637</v>
       </c>
-      <c r="C2" s="24" t="n">
+      <c r="C2" s="23" t="n">
         <v>45672</v>
       </c>
       <c r="D2" s="2" t="b">
@@ -14768,13 +15090,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="24" t="n">
+      <c r="B3" s="23" t="n">
         <v>45673</v>
       </c>
-      <c r="C3" s="24" t="n">
+      <c r="C3" s="23" t="n">
         <v>45701</v>
       </c>
       <c r="D3" s="2" t="n">
@@ -14786,10 +15108,10 @@
       <c r="A4" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="18" t="n">
+      <c r="B4" s="21" t="n">
         <v>45702</v>
       </c>
-      <c r="C4" s="18" t="n">
+      <c r="C4" s="21" t="n">
         <v>45732</v>
       </c>
       <c r="D4" s="2" t="n">
@@ -14801,10 +15123,10 @@
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="18" t="n">
+      <c r="B5" s="21" t="n">
         <v>45733</v>
       </c>
-      <c r="C5" s="18" t="n">
+      <c r="C5" s="21" t="n">
         <v>45761</v>
       </c>
       <c r="D5" s="2" t="n">
@@ -14816,10 +15138,10 @@
       <c r="A6" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="18" t="n">
+      <c r="B6" s="21" t="n">
         <v>45762</v>
       </c>
-      <c r="C6" s="18" t="n">
+      <c r="C6" s="21" t="n">
         <v>45795</v>
       </c>
       <c r="D6" s="2" t="n">
@@ -14831,10 +15153,10 @@
       <c r="A7" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="18" t="n">
+      <c r="B7" s="21" t="n">
         <v>45796</v>
       </c>
-      <c r="C7" s="18" t="n">
+      <c r="C7" s="21" t="n">
         <v>45826</v>
       </c>
       <c r="D7" s="2" t="n">
@@ -14849,7 +15171,7 @@
       <c r="B8" s="6" t="n">
         <v>45827</v>
       </c>
-      <c r="C8" s="18" t="n">
+      <c r="C8" s="21" t="n">
         <v>45855</v>
       </c>
       <c r="D8" s="2" t="n">
@@ -14861,10 +15183,10 @@
       <c r="A9" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="18" t="n">
+      <c r="B9" s="21" t="n">
         <v>45856</v>
       </c>
-      <c r="C9" s="18" t="n">
+      <c r="C9" s="21" t="n">
         <v>45886</v>
       </c>
       <c r="D9" s="2" t="n">

</xml_diff>

<commit_message>
Give invoicing periods the shorter names
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -787,40 +787,40 @@
     <t xml:space="preserve">Upper</t>
   </si>
   <si>
-    <t xml:space="preserve">January.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">February.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">March.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">May.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">June.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">August.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">October.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">November.2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">December.2025</t>
+    <t xml:space="preserve">Jan.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apr.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jun.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jul.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aug.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sep.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oct.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nov.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec.25</t>
   </si>
   <si>
     <t xml:space="preserve">Period</t>
@@ -1002,7 +1002,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1091,7 +1091,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1590,14 +1594,14 @@
   </sheetPr>
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="13.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="11.57"/>
   </cols>
@@ -1628,7 +1632,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -1651,7 +1655,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -1664,7 +1668,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B3) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1674,7 +1678,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -1687,7 +1691,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B4) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1697,7 +1701,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -1710,7 +1714,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B5) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1720,7 +1724,7 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -1733,7 +1737,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B6) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1743,7 +1747,7 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -1756,7 +1760,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B7) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1766,7 +1770,7 @@
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -1779,7 +1783,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B8) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1789,7 +1793,7 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -1802,7 +1806,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B9) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1812,7 +1816,7 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -1825,7 +1829,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B10) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1835,7 +1839,7 @@
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -1848,7 +1852,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B11) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1858,7 +1862,7 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -1871,7 +1875,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A12) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B12) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1881,7 +1885,7 @@
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -1894,7 +1898,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A13) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B13) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1904,7 +1908,7 @@
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -1917,7 +1921,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A14) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B14) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1927,7 +1931,7 @@
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -1940,7 +1944,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A15) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B15) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1950,7 +1954,7 @@
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C16" s="1" t="n">
@@ -1963,7 +1967,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A16) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B16) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1973,7 +1977,7 @@
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C17" s="1" t="n">
@@ -1986,7 +1990,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A17) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B17) &gt; 0</f>
         <v>1</v>
       </c>
@@ -1996,7 +2000,7 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C18" s="1" t="n">
@@ -2009,7 +2013,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A18) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B18) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2019,7 +2023,7 @@
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
@@ -2032,7 +2036,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A19) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B19) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2042,7 +2046,7 @@
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C20" s="1" t="n">
@@ -2055,7 +2059,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A20) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B20) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2065,7 +2069,7 @@
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C21" s="1" t="n">
@@ -2078,7 +2082,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A21) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B21) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2088,7 +2092,7 @@
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C22" s="1" t="n">
@@ -2101,7 +2105,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A22) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B22) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2111,7 +2115,7 @@
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C23" s="1" t="n">
@@ -2124,7 +2128,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A23) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F23" s="2" t="n">
+      <c r="F23" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B23) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2134,7 +2138,7 @@
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C24" s="1" t="n">
@@ -2147,7 +2151,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A24) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F24" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B24) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2157,7 +2161,7 @@
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C25" s="1" t="n">
@@ -2170,7 +2174,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A25) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B25) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2180,7 +2184,7 @@
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C26" s="1" t="n">
@@ -2193,7 +2197,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A26) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F26" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B26) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2203,7 +2207,7 @@
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C27" s="1" t="n">
@@ -2216,7 +2220,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A27) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F27" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B27) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2226,7 +2230,7 @@
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C28" s="1" t="n">
@@ -2239,7 +2243,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A28) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F28" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B28) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2249,7 +2253,7 @@
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C29" s="1" t="n">
@@ -2262,7 +2266,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A29) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F29" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B29) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2272,7 +2276,7 @@
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C30" s="1" t="n">
@@ -2285,7 +2289,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A30) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F30" s="2" t="n">
+      <c r="F30" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B30) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2295,7 +2299,7 @@
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C31" s="1" t="n">
@@ -2308,7 +2312,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A31) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F31" s="2" t="n">
+      <c r="F31" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B31) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2318,7 +2322,7 @@
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C32" s="1" t="n">
@@ -2331,7 +2335,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A32) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F32" s="2" t="n">
+      <c r="F32" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B32) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2341,7 +2345,7 @@
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C33" s="1" t="n">
@@ -2354,7 +2358,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A33) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F33" s="2" t="n">
+      <c r="F33" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B33) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2364,7 +2368,7 @@
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C34" s="1" t="n">
@@ -2377,7 +2381,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A34) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F34" s="2" t="n">
+      <c r="F34" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B34) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2387,7 +2391,7 @@
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C35" s="1" t="n">
@@ -2400,7 +2404,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A35) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F35" s="2" t="n">
+      <c r="F35" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B35) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2410,7 +2414,7 @@
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C36" s="1" t="n">
@@ -2423,7 +2427,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A36) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="F36" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B36) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2432,7 +2436,7 @@
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C37" s="1" t="n">
@@ -2445,7 +2449,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A37) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="F37" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B37) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2454,7 +2458,7 @@
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C38" s="1" t="n">
@@ -2467,7 +2471,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A38) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F38" s="2" t="n">
+      <c r="F38" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B38) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2476,7 +2480,7 @@
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C39" s="1" t="n">
@@ -2489,7 +2493,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A39) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F39" s="2" t="n">
+      <c r="F39" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B39) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2498,7 +2502,7 @@
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C40" s="1" t="n">
@@ -2511,7 +2515,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A40) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F40" s="2" t="n">
+      <c r="F40" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B40) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2520,7 +2524,7 @@
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C41" s="1" t="n">
@@ -2533,7 +2537,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A41) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F41" s="2" t="n">
+      <c r="F41" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B41) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2542,7 +2546,7 @@
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C42" s="1" t="n">
@@ -2555,7 +2559,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A42) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F42" s="2" t="n">
+      <c r="F42" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B42) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2564,7 +2568,7 @@
       <c r="A43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C43" s="1" t="n">
@@ -2577,7 +2581,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A43) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F43" s="2" t="n">
+      <c r="F43" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B43) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2586,7 +2590,7 @@
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C44" s="1" t="n">
@@ -2599,7 +2603,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A44) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F44" s="2" t="n">
+      <c r="F44" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B44) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2608,7 +2612,7 @@
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C45" s="1" t="n">
@@ -2621,7 +2625,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A45) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F45" s="2" t="n">
+      <c r="F45" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B45) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2630,7 +2634,7 @@
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C46" s="1" t="n">
@@ -2643,7 +2647,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A46) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F46" s="2" t="n">
+      <c r="F46" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B46) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2652,7 +2656,7 @@
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C47" s="1" t="n">
@@ -2665,7 +2669,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A47) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F47" s="2" t="n">
+      <c r="F47" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B47) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2674,7 +2678,7 @@
       <c r="A48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C48" s="1" t="n">
@@ -2687,7 +2691,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A48) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F48" s="2" t="n">
+      <c r="F48" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B48) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2696,7 +2700,7 @@
       <c r="A49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C49" s="1" t="n">
@@ -2709,7 +2713,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A49) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F49" s="2" t="n">
+      <c r="F49" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B49) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2718,7 +2722,7 @@
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C50" s="1" t="n">
@@ -2731,7 +2735,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A50) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F50" s="2" t="n">
+      <c r="F50" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B50) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2740,7 +2744,7 @@
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C51" s="1" t="n">
@@ -2753,7 +2757,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A51) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F51" s="2" t="n">
+      <c r="F51" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B51) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2762,7 +2766,7 @@
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C52" s="1" t="n">
@@ -2775,7 +2779,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A52) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F52" s="2" t="n">
+      <c r="F52" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B52) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2784,7 +2788,7 @@
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C53" s="1" t="n">
@@ -2797,7 +2801,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A53) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F53" s="2" t="n">
+      <c r="F53" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B53) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2806,7 +2810,7 @@
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C54" s="1" t="n">
@@ -2819,7 +2823,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A54) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F54" s="2" t="n">
+      <c r="F54" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B54) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2828,7 +2832,7 @@
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C55" s="1" t="n">
@@ -2841,7 +2845,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A55) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F55" s="2" t="n">
+      <c r="F55" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B55) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2850,7 +2854,7 @@
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C56" s="1" t="n">
@@ -2863,7 +2867,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A56) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F56" s="2" t="n">
+      <c r="F56" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B56) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2872,7 +2876,7 @@
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C57" s="1" t="n">
@@ -2885,7 +2889,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A57) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F57" s="2" t="n">
+      <c r="F57" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B57) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2894,7 +2898,7 @@
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C58" s="1" t="n">
@@ -2907,7 +2911,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A58) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F58" s="2" t="n">
+      <c r="F58" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B58) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2916,7 +2920,7 @@
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C59" s="1" t="n">
@@ -2929,7 +2933,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A59) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F59" s="2" t="n">
+      <c r="F59" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B59) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2938,7 +2942,7 @@
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C60" s="1" t="n">
@@ -2951,7 +2955,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A60) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F60" s="2" t="n">
+      <c r="F60" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B60) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2960,7 +2964,7 @@
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C61" s="1" t="n">
@@ -2973,7 +2977,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A61) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F61" s="2" t="n">
+      <c r="F61" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B61) &gt; 0</f>
         <v>1</v>
       </c>
@@ -2982,7 +2986,7 @@
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C62" s="1" t="n">
@@ -2995,7 +2999,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A62) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F62" s="2" t="n">
+      <c r="F62" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B62) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3004,7 +3008,7 @@
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C63" s="1" t="n">
@@ -3017,7 +3021,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A63) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F63" s="2" t="n">
+      <c r="F63" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B63) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3026,7 +3030,7 @@
       <c r="A64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C64" s="1" t="n">
@@ -3039,7 +3043,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A64) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F64" s="2" t="n">
+      <c r="F64" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B64) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3048,7 +3052,7 @@
       <c r="A65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C65" s="1" t="n">
@@ -3061,7 +3065,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A65) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F65" s="2" t="n">
+      <c r="F65" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B65) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3070,7 +3074,7 @@
       <c r="A66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C66" s="1" t="n">
@@ -3083,7 +3087,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A66) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F66" s="2" t="n">
+      <c r="F66" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B66) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3092,7 +3096,7 @@
       <c r="A67" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C67" s="1" t="n">
@@ -3105,7 +3109,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A67) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F67" s="2" t="n">
+      <c r="F67" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B67) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3114,7 +3118,7 @@
       <c r="A68" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C68" s="1" t="n">
@@ -3127,7 +3131,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A68) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F68" s="2" t="n">
+      <c r="F68" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B68) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3136,7 +3140,7 @@
       <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C69" s="1" t="n">
@@ -3149,7 +3153,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A69) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F69" s="2" t="n">
+      <c r="F69" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B69) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3158,7 +3162,7 @@
       <c r="A70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C70" s="1" t="n">
@@ -3171,7 +3175,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A70) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F70" s="2" t="n">
+      <c r="F70" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B70) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3180,7 +3184,7 @@
       <c r="A71" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C71" s="1" t="n">
@@ -3193,7 +3197,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A71) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F71" s="2" t="n">
+      <c r="F71" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B71) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3202,7 +3206,7 @@
       <c r="A72" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C72" s="1" t="n">
@@ -3215,7 +3219,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A72) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F72" s="2" t="n">
+      <c r="F72" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B72) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3224,7 +3228,7 @@
       <c r="A73" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C73" s="1" t="n">
@@ -3237,7 +3241,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A73) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F73" s="2" t="n">
+      <c r="F73" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B73) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3246,7 +3250,7 @@
       <c r="A74" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C74" s="1" t="n">
@@ -3259,7 +3263,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A74) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F74" s="2" t="n">
+      <c r="F74" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B74) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3268,7 +3272,7 @@
       <c r="A75" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="22" t="s">
+      <c r="B75" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C75" s="1" t="n">
@@ -3281,7 +3285,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A75) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F75" s="2" t="n">
+      <c r="F75" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B75) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3290,7 +3294,7 @@
       <c r="A76" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C76" s="1" t="n">
@@ -3303,7 +3307,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A76) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F76" s="2" t="n">
+      <c r="F76" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B76) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3312,7 +3316,7 @@
       <c r="A77" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C77" s="1" t="n">
@@ -3325,7 +3329,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A77) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F77" s="2" t="n">
+      <c r="F77" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B77) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3334,7 +3338,7 @@
       <c r="A78" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C78" s="1" t="n">
@@ -3347,7 +3351,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A78) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F78" s="2" t="n">
+      <c r="F78" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B78) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3356,7 +3360,7 @@
       <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C79" s="1" t="n">
@@ -3369,7 +3373,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A79) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F79" s="2" t="n">
+      <c r="F79" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B79) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3378,7 +3382,7 @@
       <c r="A80" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C80" s="1" t="n">
@@ -3391,7 +3395,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A80) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F80" s="2" t="n">
+      <c r="F80" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B80) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3400,7 +3404,7 @@
       <c r="A81" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C81" s="1" t="n">
@@ -3413,7 +3417,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A81) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F81" s="2" t="n">
+      <c r="F81" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B81) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3422,7 +3426,7 @@
       <c r="A82" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C82" s="1" t="n">
@@ -3435,7 +3439,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A82) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F82" s="2" t="n">
+      <c r="F82" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B82) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3444,7 +3448,7 @@
       <c r="A83" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C83" s="1" t="n">
@@ -3457,7 +3461,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A83) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F83" s="2" t="n">
+      <c r="F83" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B83) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3466,7 +3470,7 @@
       <c r="A84" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C84" s="1" t="n">
@@ -3479,7 +3483,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A84) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F84" s="2" t="n">
+      <c r="F84" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B84) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3488,7 +3492,7 @@
       <c r="A85" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C85" s="1" t="n">
@@ -3501,7 +3505,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A85) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F85" s="2" t="n">
+      <c r="F85" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B85) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3510,7 +3514,7 @@
       <c r="A86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B86" s="22" t="s">
+      <c r="B86" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C86" s="1" t="n">
@@ -3523,7 +3527,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A86) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F86" s="2" t="n">
+      <c r="F86" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B86) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3532,7 +3536,7 @@
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="22" t="s">
+      <c r="B87" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C87" s="1" t="n">
@@ -3545,7 +3549,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A87) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F87" s="2" t="n">
+      <c r="F87" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B87) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3554,7 +3558,7 @@
       <c r="A88" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C88" s="1" t="n">
@@ -3567,7 +3571,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A88) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F88" s="2" t="n">
+      <c r="F88" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B88) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3576,7 +3580,7 @@
       <c r="A89" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C89" s="1" t="n">
@@ -3589,7 +3593,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A89) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F89" s="2" t="n">
+      <c r="F89" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B89) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3598,7 +3602,7 @@
       <c r="A90" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C90" s="1" t="n">
@@ -3611,7 +3615,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A90) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F90" s="2" t="n">
+      <c r="F90" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B90) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3620,7 +3624,7 @@
       <c r="A91" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C91" s="1" t="n">
@@ -3633,7 +3637,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A91) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F91" s="2" t="n">
+      <c r="F91" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B91) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3642,7 +3646,7 @@
       <c r="A92" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C92" s="1" t="n">
@@ -3655,7 +3659,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A92) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F92" s="2" t="n">
+      <c r="F92" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B92) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3664,7 +3668,7 @@
       <c r="A93" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C93" s="1" t="n">
@@ -3677,7 +3681,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A93) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F93" s="2" t="n">
+      <c r="F93" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B93) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3686,7 +3690,7 @@
       <c r="A94" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C94" s="1" t="n">
@@ -3699,7 +3703,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A94) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F94" s="2" t="n">
+      <c r="F94" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B94) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3708,7 +3712,7 @@
       <c r="A95" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C95" s="1" t="n">
@@ -3721,7 +3725,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A95) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F95" s="2" t="n">
+      <c r="F95" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B95) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3730,7 +3734,7 @@
       <c r="A96" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C96" s="1" t="n">
@@ -3743,7 +3747,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A96) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F96" s="2" t="n">
+      <c r="F96" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B96) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3752,7 +3756,7 @@
       <c r="A97" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C97" s="1" t="n">
@@ -3765,7 +3769,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A97) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F97" s="2" t="n">
+      <c r="F97" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B97) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3774,7 +3778,7 @@
       <c r="A98" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B98" s="22" t="s">
+      <c r="B98" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C98" s="1" t="n">
@@ -3787,7 +3791,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A98) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F98" s="2" t="n">
+      <c r="F98" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B98) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3796,7 +3800,7 @@
       <c r="A99" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C99" s="1" t="n">
@@ -3809,7 +3813,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A99) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F99" s="2" t="n">
+      <c r="F99" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B99) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3818,7 +3822,7 @@
       <c r="A100" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C100" s="1" t="n">
@@ -3831,7 +3835,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A100) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F100" s="2" t="n">
+      <c r="F100" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B100) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3840,7 +3844,7 @@
       <c r="A101" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C101" s="1" t="n">
@@ -3853,7 +3857,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A101) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F101" s="2" t="n">
+      <c r="F101" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B101) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3862,7 +3866,7 @@
       <c r="A102" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C102" s="1" t="n">
@@ -3875,7 +3879,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A102) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F102" s="2" t="n">
+      <c r="F102" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B102) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3884,7 +3888,7 @@
       <c r="A103" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C103" s="1" t="n">
@@ -3897,7 +3901,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A103) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F103" s="2" t="n">
+      <c r="F103" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B103) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3906,7 +3910,7 @@
       <c r="A104" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C104" s="1" t="n">
@@ -3919,7 +3923,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A104) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F104" s="2" t="n">
+      <c r="F104" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B104) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3928,7 +3932,7 @@
       <c r="A105" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C105" s="1" t="n">
@@ -3941,7 +3945,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A105) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F105" s="2" t="n">
+      <c r="F105" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B105) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3950,7 +3954,7 @@
       <c r="A106" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C106" s="1" t="n">
@@ -3963,7 +3967,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A106) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F106" s="2" t="n">
+      <c r="F106" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B106) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3972,7 +3976,7 @@
       <c r="A107" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C107" s="1" t="n">
@@ -3985,7 +3989,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A107) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F107" s="2" t="n">
+      <c r="F107" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B107) &gt; 0</f>
         <v>1</v>
       </c>
@@ -3994,7 +3998,7 @@
       <c r="A108" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C108" s="1" t="n">
@@ -4007,7 +4011,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A108) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F108" s="2" t="n">
+      <c r="F108" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B108) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4016,7 +4020,7 @@
       <c r="A109" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C109" s="1" t="n">
@@ -4029,7 +4033,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A109) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F109" s="2" t="n">
+      <c r="F109" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B109) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4038,7 +4042,7 @@
       <c r="A110" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B110" s="22" t="s">
+      <c r="B110" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C110" s="1" t="n">
@@ -4051,7 +4055,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A110) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F110" s="2" t="n">
+      <c r="F110" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B110) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4060,7 +4064,7 @@
       <c r="A111" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="22" t="s">
+      <c r="B111" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C111" s="1" t="n">
@@ -4073,7 +4077,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A111) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F111" s="2" t="n">
+      <c r="F111" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B111) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4082,7 +4086,7 @@
       <c r="A112" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C112" s="1" t="n">
@@ -4095,7 +4099,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A112) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F112" s="2" t="n">
+      <c r="F112" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B112) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4104,7 +4108,7 @@
       <c r="A113" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C113" s="1" t="n">
@@ -4117,7 +4121,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A113) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F113" s="2" t="n">
+      <c r="F113" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B113) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4126,7 +4130,7 @@
       <c r="A114" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C114" s="1" t="n">
@@ -4139,7 +4143,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A114) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F114" s="2" t="n">
+      <c r="F114" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B114) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4148,7 +4152,7 @@
       <c r="A115" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C115" s="1" t="n">
@@ -4161,7 +4165,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A115) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F115" s="2" t="n">
+      <c r="F115" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B115) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4170,7 +4174,7 @@
       <c r="A116" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C116" s="1" t="n">
@@ -4183,7 +4187,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A116) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F116" s="2" t="n">
+      <c r="F116" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B116) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4192,7 +4196,7 @@
       <c r="A117" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C117" s="1" t="n">
@@ -4205,7 +4209,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A117) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F117" s="2" t="n">
+      <c r="F117" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B117) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4214,7 +4218,7 @@
       <c r="A118" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C118" s="1" t="n">
@@ -4227,7 +4231,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A118) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F118" s="2" t="n">
+      <c r="F118" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B118) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4236,7 +4240,7 @@
       <c r="A119" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C119" s="1" t="n">
@@ -4249,7 +4253,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A119) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F119" s="2" t="n">
+      <c r="F119" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B119) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4258,7 +4262,7 @@
       <c r="A120" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C120" s="1" t="n">
@@ -4271,7 +4275,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A120) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F120" s="2" t="n">
+      <c r="F120" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B120) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4280,7 +4284,7 @@
       <c r="A121" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C121" s="1" t="n">
@@ -4293,7 +4297,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A121) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F121" s="2" t="n">
+      <c r="F121" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B121) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4302,7 +4306,7 @@
       <c r="A122" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B122" s="22" t="s">
+      <c r="B122" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C122" s="1" t="n">
@@ -4315,7 +4319,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A122) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F122" s="2" t="n">
+      <c r="F122" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B122) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4324,7 +4328,7 @@
       <c r="A123" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B123" s="22" t="s">
+      <c r="B123" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C123" s="1" t="n">
@@ -4337,7 +4341,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A123) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F123" s="2" t="n">
+      <c r="F123" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B123) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4346,7 +4350,7 @@
       <c r="A124" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C124" s="1" t="n">
@@ -4359,7 +4363,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A124) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F124" s="2" t="n">
+      <c r="F124" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B124) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4368,7 +4372,7 @@
       <c r="A125" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C125" s="1" t="n">
@@ -4381,7 +4385,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A125) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F125" s="2" t="n">
+      <c r="F125" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B125) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4390,7 +4394,7 @@
       <c r="A126" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C126" s="1" t="n">
@@ -4403,7 +4407,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A126) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F126" s="2" t="n">
+      <c r="F126" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B126) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4412,7 +4416,7 @@
       <c r="A127" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C127" s="1" t="n">
@@ -4425,7 +4429,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A127) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F127" s="2" t="n">
+      <c r="F127" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B127) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4434,7 +4438,7 @@
       <c r="A128" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C128" s="1" t="n">
@@ -4447,7 +4451,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A128) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F128" s="2" t="n">
+      <c r="F128" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B128) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4456,7 +4460,7 @@
       <c r="A129" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C129" s="1" t="n">
@@ -4469,7 +4473,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A129) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F129" s="2" t="n">
+      <c r="F129" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B129) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4478,7 +4482,7 @@
       <c r="A130" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C130" s="1" t="n">
@@ -4491,7 +4495,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A130) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F130" s="2" t="n">
+      <c r="F130" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B130) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4500,7 +4504,7 @@
       <c r="A131" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C131" s="1" t="n">
@@ -4513,7 +4517,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A131) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F131" s="2" t="n">
+      <c r="F131" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B131) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4522,7 +4526,7 @@
       <c r="A132" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C132" s="1" t="n">
@@ -4535,7 +4539,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A132) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F132" s="2" t="n">
+      <c r="F132" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B132) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4544,7 +4548,7 @@
       <c r="A133" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C133" s="1" t="n">
@@ -4557,7 +4561,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A133) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F133" s="2" t="n">
+      <c r="F133" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B133) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4566,7 +4570,7 @@
       <c r="A134" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B134" s="22" t="s">
+      <c r="B134" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C134" s="1" t="n">
@@ -4579,7 +4583,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A134) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F134" s="2" t="n">
+      <c r="F134" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B134) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4588,7 +4592,7 @@
       <c r="A135" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B135" s="22" t="s">
+      <c r="B135" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C135" s="1" t="n">
@@ -4601,7 +4605,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A135) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F135" s="2" t="n">
+      <c r="F135" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B135) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4610,7 +4614,7 @@
       <c r="A136" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C136" s="1" t="n">
@@ -4623,7 +4627,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A136) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F136" s="2" t="n">
+      <c r="F136" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B136) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4633,7 +4637,7 @@
       <c r="A137" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C137" s="1" t="n">
@@ -4646,7 +4650,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A137) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F137" s="2" t="n">
+      <c r="F137" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B137) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4656,7 +4660,7 @@
       <c r="A138" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C138" s="1" t="n">
@@ -4669,7 +4673,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A138) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F138" s="2" t="n">
+      <c r="F138" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B138) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4679,7 +4683,7 @@
       <c r="A139" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C139" s="1" t="n">
@@ -4692,7 +4696,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A139) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F139" s="2" t="n">
+      <c r="F139" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B139) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4702,7 +4706,7 @@
       <c r="A140" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C140" s="1" t="n">
@@ -4715,7 +4719,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A140) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F140" s="2" t="n">
+      <c r="F140" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B140) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4725,7 +4729,7 @@
       <c r="A141" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C141" s="1" t="n">
@@ -4738,7 +4742,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A141) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F141" s="2" t="n">
+      <c r="F141" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B141) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4748,7 +4752,7 @@
       <c r="A142" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C142" s="1" t="n">
@@ -4761,7 +4765,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A142) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F142" s="2" t="n">
+      <c r="F142" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B142) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4771,7 +4775,7 @@
       <c r="A143" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C143" s="1" t="n">
@@ -4784,7 +4788,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A143) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F143" s="2" t="n">
+      <c r="F143" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B143) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4794,7 +4798,7 @@
       <c r="A144" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C144" s="1" t="n">
@@ -4807,7 +4811,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A144) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F144" s="2" t="n">
+      <c r="F144" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B144) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4816,7 +4820,7 @@
       <c r="A145" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C145" s="1" t="n">
@@ -4829,7 +4833,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A145) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F145" s="2" t="n">
+      <c r="F145" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B145) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4838,7 +4842,7 @@
       <c r="A146" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B146" s="22" t="s">
+      <c r="B146" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C146" s="1" t="n">
@@ -4851,7 +4855,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A146) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F146" s="2" t="n">
+      <c r="F146" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B146) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4860,7 +4864,7 @@
       <c r="A147" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B147" s="22" t="s">
+      <c r="B147" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C147" s="1" t="n">
@@ -4873,7 +4877,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A147) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F147" s="2" t="n">
+      <c r="F147" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B147) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4882,7 +4886,7 @@
       <c r="A148" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C148" s="1" t="n">
@@ -4895,7 +4899,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A148) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F148" s="2" t="n">
+      <c r="F148" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B148) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4904,7 +4908,7 @@
       <c r="A149" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C149" s="1" t="n">
@@ -4917,7 +4921,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A149) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F149" s="2" t="n">
+      <c r="F149" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B149) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4926,7 +4930,7 @@
       <c r="A150" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C150" s="1" t="n">
@@ -4939,7 +4943,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A150) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F150" s="2" t="n">
+      <c r="F150" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B150) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4948,7 +4952,7 @@
       <c r="A151" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C151" s="1" t="n">
@@ -4961,7 +4965,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A151) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F151" s="2" t="n">
+      <c r="F151" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B151) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4970,7 +4974,7 @@
       <c r="A152" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C152" s="1" t="n">
@@ -4983,7 +4987,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A152) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F152" s="2" t="n">
+      <c r="F152" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B152) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4992,7 +4996,7 @@
       <c r="A153" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C153" s="1" t="n">
@@ -5005,7 +5009,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A153) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F153" s="2" t="n">
+      <c r="F153" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B153) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5014,7 +5018,7 @@
       <c r="A154" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B154" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C154" s="1" t="n">
@@ -5027,7 +5031,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A154) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F154" s="2" t="n">
+      <c r="F154" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B154) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5036,7 +5040,7 @@
       <c r="A155" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B155" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C155" s="1" t="n">
@@ -5049,7 +5053,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A155) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F155" s="2" t="n">
+      <c r="F155" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B155) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5058,7 +5062,7 @@
       <c r="A156" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B156" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C156" s="1" t="n">
@@ -5071,7 +5075,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A156) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F156" s="2" t="n">
+      <c r="F156" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B156) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5080,7 +5084,7 @@
       <c r="A157" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B157" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C157" s="1" t="n">
@@ -5093,7 +5097,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A157) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F157" s="2" t="n">
+      <c r="F157" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B157) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5102,7 +5106,7 @@
       <c r="A158" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B158" s="22" t="s">
+      <c r="B158" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C158" s="1" t="n">
@@ -5115,7 +5119,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A158) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F158" s="2" t="n">
+      <c r="F158" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B158) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5124,7 +5128,7 @@
       <c r="A159" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B159" s="22" t="s">
+      <c r="B159" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C159" s="1" t="n">
@@ -5137,7 +5141,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A159) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F159" s="2" t="n">
+      <c r="F159" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B159) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5146,7 +5150,7 @@
       <c r="A160" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C160" s="1" t="n">
@@ -5159,7 +5163,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A160) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F160" s="2" t="n">
+      <c r="F160" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B160) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5168,7 +5172,7 @@
       <c r="A161" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C161" s="1" t="n">
@@ -5181,7 +5185,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A161) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F161" s="2" t="n">
+      <c r="F161" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B161) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5190,7 +5194,7 @@
       <c r="A162" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C162" s="1" t="n">
@@ -5203,7 +5207,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A162) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F162" s="2" t="n">
+      <c r="F162" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B162) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5212,7 +5216,7 @@
       <c r="A163" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C163" s="1" t="n">
@@ -5225,7 +5229,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A163) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F163" s="2" t="n">
+      <c r="F163" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B163) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5234,7 +5238,7 @@
       <c r="A164" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C164" s="1" t="n">
@@ -5247,7 +5251,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A164) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F164" s="2" t="n">
+      <c r="F164" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B164) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5256,7 +5260,7 @@
       <c r="A165" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C165" s="1" t="n">
@@ -5269,7 +5273,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A165) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F165" s="2" t="n">
+      <c r="F165" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B165) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5278,7 +5282,7 @@
       <c r="A166" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C166" s="1" t="n">
@@ -5291,7 +5295,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A166) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F166" s="2" t="n">
+      <c r="F166" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B166) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5300,7 +5304,7 @@
       <c r="A167" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C167" s="1" t="n">
@@ -5313,7 +5317,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A167) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F167" s="2" t="n">
+      <c r="F167" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B167) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5322,7 +5326,7 @@
       <c r="A168" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C168" s="1" t="n">
@@ -5335,7 +5339,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A168) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F168" s="2" t="n">
+      <c r="F168" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B168) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5344,7 +5348,7 @@
       <c r="A169" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C169" s="1" t="n">
@@ -5357,7 +5361,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A169) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F169" s="2" t="n">
+      <c r="F169" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B169) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5366,7 +5370,7 @@
       <c r="A170" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B170" s="22" t="s">
+      <c r="B170" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C170" s="1" t="n">
@@ -5379,7 +5383,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A170) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F170" s="2" t="n">
+      <c r="F170" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B170) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5388,7 +5392,7 @@
       <c r="A171" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B171" s="22" t="s">
+      <c r="B171" s="23" t="s">
         <v>131</v>
       </c>
       <c r="C171" s="1" t="n">
@@ -5401,7 +5405,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A171) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F171" s="2" t="n">
+      <c r="F171" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B171) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5410,7 +5414,7 @@
       <c r="A172" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B172" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C172" s="1" t="n">
@@ -5423,7 +5427,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A172) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F172" s="2" t="n">
+      <c r="F172" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B172) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5432,7 +5436,7 @@
       <c r="A173" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B173" s="22" t="s">
         <v>133</v>
       </c>
       <c r="C173" s="1" t="n">
@@ -5445,7 +5449,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A173) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F173" s="2" t="n">
+      <c r="F173" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B173) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5454,7 +5458,7 @@
       <c r="A174" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B174" s="22" t="s">
         <v>134</v>
       </c>
       <c r="C174" s="1" t="n">
@@ -5467,7 +5471,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A174) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F174" s="2" t="n">
+      <c r="F174" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B174) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5476,7 +5480,7 @@
       <c r="A175" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="B175" s="22" t="s">
         <v>135</v>
       </c>
       <c r="C175" s="1" t="n">
@@ -5489,7 +5493,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A175) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F175" s="2" t="n">
+      <c r="F175" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B175) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5498,7 +5502,7 @@
       <c r="A176" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B176" s="22" t="s">
         <v>136</v>
       </c>
       <c r="C176" s="1" t="n">
@@ -5511,7 +5515,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A176) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F176" s="2" t="n">
+      <c r="F176" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B176) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5520,7 +5524,7 @@
       <c r="A177" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="B177" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C177" s="1" t="n">
@@ -5533,7 +5537,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A177) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F177" s="2" t="n">
+      <c r="F177" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B177) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5542,7 +5546,7 @@
       <c r="A178" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="B178" s="22" t="s">
         <v>138</v>
       </c>
       <c r="C178" s="1" t="n">
@@ -5555,7 +5559,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A178) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F178" s="2" t="n">
+      <c r="F178" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B178) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5564,7 +5568,7 @@
       <c r="A179" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B179" s="1" t="s">
+      <c r="B179" s="22" t="s">
         <v>139</v>
       </c>
       <c r="C179" s="1" t="n">
@@ -5577,7 +5581,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A179) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F179" s="2" t="n">
+      <c r="F179" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B179) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5586,7 +5590,7 @@
       <c r="A180" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B180" s="22" t="s">
         <v>140</v>
       </c>
       <c r="C180" s="1" t="n">
@@ -5599,7 +5603,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A180) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F180" s="2" t="n">
+      <c r="F180" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B180) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5608,7 +5612,7 @@
       <c r="A181" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B181" s="22" t="s">
         <v>141</v>
       </c>
       <c r="C181" s="1" t="n">
@@ -5621,7 +5625,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A181) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F181" s="2" t="n">
+      <c r="F181" s="2" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B181) &gt; 0</f>
         <v>1</v>
       </c>
@@ -5874,19 +5878,19 @@
       <c r="H1" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="26" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5915,23 +5919,23 @@
       <c r="H2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I2" s="26" t="n">
+      <c r="I2" s="27" t="n">
         <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C900))</f>
         <v>46053</v>
       </c>
-      <c r="J2" s="27" t="n">
+      <c r="J2" s="28" t="n">
         <f aca="false">AND(ISNUMBER(D2), D2&gt;A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="28" t="b">
+      <c r="K2" s="29" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&lt;=I2)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="28" t="b">
+      <c r="L2" s="29" t="b">
         <f aca="false">AND(ISNUMBER(F2), F2&gt;A2)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="28" t="b">
+      <c r="M2" s="29" t="b">
         <f aca="false">AND(ISNUMBER(G2), G2&lt;=I2)</f>
         <v>1</v>
       </c>
@@ -11388,7 +11392,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
     </sheetView>
   </sheetViews>
@@ -15049,18 +15053,18 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="22" width="21.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="7" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -15075,13 +15079,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="24" t="n">
         <v>45637</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="24" t="n">
         <v>45672</v>
       </c>
       <c r="D2" s="2" t="b">
@@ -15090,13 +15094,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="24" t="n">
         <v>45673</v>
       </c>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="24" t="n">
         <v>45701</v>
       </c>
       <c r="D3" s="2" t="n">
@@ -15105,7 +15109,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="22" t="s">
         <v>132</v>
       </c>
       <c r="B4" s="21" t="n">
@@ -15120,7 +15124,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="22" t="s">
         <v>133</v>
       </c>
       <c r="B5" s="21" t="n">
@@ -15135,7 +15139,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="22" t="s">
         <v>134</v>
       </c>
       <c r="B6" s="21" t="n">
@@ -15150,7 +15154,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="22" t="s">
         <v>135</v>
       </c>
       <c r="B7" s="21" t="n">
@@ -15165,7 +15169,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="22" t="s">
         <v>136</v>
       </c>
       <c r="B8" s="6" t="n">
@@ -15180,7 +15184,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="22" t="s">
         <v>137</v>
       </c>
       <c r="B9" s="21" t="n">
@@ -15195,7 +15199,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="22" t="s">
         <v>138</v>
       </c>
       <c r="B10" s="6" t="n">
@@ -15210,7 +15214,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="22" t="s">
         <v>139</v>
       </c>
       <c r="B11" s="6" t="n">
@@ -15225,7 +15229,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="22" t="s">
         <v>140</v>
       </c>
       <c r="B12" s="6" t="n">
@@ -15240,7 +15244,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="22" t="s">
         <v>141</v>
       </c>
       <c r="B13" s="6" t="n">

</xml_diff>

<commit_message>
Add addtional input data verification in example 09
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -79,6 +79,29 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Valid period?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Are dates OK?</t>
         </r>
       </text>
     </comment>
@@ -1002,7 +1025,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1105,6 +1128,10 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1309,7 +1336,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1594,8 +1621,8 @@
   </sheetPr>
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5647,50 +5674,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
         <v>143</v>
       </c>
+      <c r="B1" s="11" t="b">
+        <f aca="false">AND(B2:B908)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
         <v>45650</v>
       </c>
+      <c r="B2" s="2" t="b">
+        <f aca="false">AND(ISNUMBER(A2),misc!$A$2&lt;=A2)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
         <v>45651</v>
       </c>
+      <c r="B3" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(A3),misc!$A$2&lt;=A3)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <v>45652</v>
       </c>
+      <c r="B4" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(A4),misc!$A$2&lt;=A4)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <v>45658</v>
       </c>
+      <c r="B5" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(A5),misc!$A$2&lt;=A5)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <v>45767</v>
       </c>
+      <c r="B6" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(A6),misc!$A$2&lt;=A6)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
         <v>45778</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <f aca="false">AND(ISNUMBER(A7),misc!$A$2&lt;=A7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5827,6 +5883,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5838,7 +5895,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5878,19 +5935,19 @@
       <c r="H1" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="27" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5919,23 +5976,23 @@
       <c r="H2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I2" s="27" t="n">
+      <c r="I2" s="28" t="n">
         <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C900))</f>
         <v>46053</v>
       </c>
-      <c r="J2" s="28" t="n">
+      <c r="J2" s="29" t="n">
         <f aca="false">AND(ISNUMBER(D2), D2&gt;A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="29" t="b">
+      <c r="K2" s="30" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&lt;=I2)</f>
         <v>1</v>
       </c>
-      <c r="L2" s="29" t="b">
+      <c r="L2" s="30" t="b">
         <f aca="false">AND(ISNUMBER(F2), F2&gt;A2)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="29" t="b">
+      <c r="M2" s="30" t="b">
         <f aca="false">AND(ISNUMBER(G2), G2&lt;=I2)</f>
         <v>1</v>
       </c>
@@ -5958,8 +6015,8 @@
   </sheetPr>
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A100" activeCellId="0" sqref="A100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11393,7 +11450,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F60" activeCellId="0" sqref="F60"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13295,7 +13352,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13716,7 +13773,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14362,7 +14419,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14783,7 +14840,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15053,7 +15110,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Set solver as GCG for examples 10,11,12,13
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -99,7 +99,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Are dates OK?</t>
         </r>
@@ -1130,7 +1129,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1336,7 +1335,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="H2 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1622,7 +1621,7 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="H2 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5676,8 +5675,8 @@
   </sheetPr>
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="H2 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5894,8 +5893,8 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6016,7 +6015,7 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="H2 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8803,7 +8802,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="H2 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11450,7 +11449,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13352,7 +13351,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13773,7 +13772,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="H2 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14419,7 +14418,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14840,7 +14839,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="H2 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15110,7 +15109,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="H2 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Delete code removeing items before TODAY. Adjust examples
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
+++ b/ampl-data-input-excel/09-experts16-tastks109/09-experts16-tastks109.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -234,52 +234,6 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author>Unknown Author</author>
-  </authors>
-  <commentList>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Valid expert?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Valid task?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Are date OK?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
@@ -299,52 +253,6 @@
       </text>
     </comment>
     <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Are date OK?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author>Unknown Author</author>
-  </authors>
-  <commentList>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Valid expert?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Valid task?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1335,7 +1243,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="H2 C1"/>
+      <selection pane="topLeft" activeCell="D78" activeCellId="0" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1621,7 +1529,7 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="H2 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5673,10 +5581,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="1" sqref="H2 D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5690,63 +5598,45 @@
         <v>143</v>
       </c>
       <c r="B1" s="11" t="b">
-        <f aca="false">AND(B2:B908)</f>
-        <v>0</v>
+        <f aca="false">AND(B2:B905)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
-        <v>45650</v>
-      </c>
-      <c r="B2" s="2" t="b">
+        <v>45658</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <f aca="false">AND(ISNUMBER(A2),misc!$A$2&lt;=A2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
-        <v>45651</v>
+        <v>45767</v>
       </c>
       <c r="B3" s="2" t="n">
         <f aca="false">AND(ISNUMBER(A3),misc!$A$2&lt;=A3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
-        <v>45652</v>
+        <v>45778</v>
       </c>
       <c r="B4" s="2" t="n">
         <f aca="false">AND(ISNUMBER(A4),misc!$A$2&lt;=A4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
-        <v>45658</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(A5),misc!$A$2&lt;=A5)</f>
-        <v>1</v>
-      </c>
+      <c r="A5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
-        <v>45767</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(A6),misc!$A$2&lt;=A6)</f>
-        <v>1</v>
-      </c>
+      <c r="A6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
-        <v>45778</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <f aca="false">AND(ISNUMBER(A7),misc!$A$2&lt;=A7)</f>
-        <v>1</v>
-      </c>
+      <c r="A7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
@@ -5865,15 +5755,9 @@
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6"/>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5893,8 +5777,8 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6015,7 +5899,7 @@
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="H2 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8802,7 +8686,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="H2 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11449,7 +11333,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13348,10 +13232,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13360,7 +13244,6 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13382,35 +13265,11 @@
       <c r="F1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="5" t="b">
-        <f aca="false">AND(G2:G938)</f>
-        <v>0</v>
-      </c>
-      <c r="H1" s="5" t="b">
-        <f aca="false">AND(H2:H938)</f>
-        <v>0</v>
-      </c>
-      <c r="I1" s="11" t="b">
-        <f aca="false">AND(I2:I908)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="1"/>
-      <c r="G2" s="2" t="b">
-        <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="b">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B2)&gt;0</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="b">
-        <f aca="false">AND(ISNUMBER(C2), ISNUMBER(D2), C2&lt;=D2)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1"/>
@@ -13760,7 +13619,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13772,7 +13630,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="H2 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14415,10 +14273,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="H2 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14427,7 +14285,6 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="2" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14449,35 +14306,11 @@
       <c r="F1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="5" t="b">
-        <f aca="false">AND(G2:G938)</f>
-        <v>0</v>
-      </c>
-      <c r="H1" s="5" t="b">
-        <f aca="false">AND(H2:H938)</f>
-        <v>0</v>
-      </c>
-      <c r="I1" s="11" t="b">
-        <f aca="false">AND(I2:I908)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="1"/>
-      <c r="G2" s="2" t="b">
-        <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="b">
-        <f aca="false">COUNTIF(tasks!$A$2:$A$903,B2)&gt;0</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="b">
-        <f aca="false">AND(ISNUMBER(C2), ISNUMBER(D2), C2&lt;=D2)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="12"/>
@@ -14827,7 +14660,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14839,7 +14671,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="H2 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15109,7 +14941,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="H2 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>